<commit_message>
feat: desc primera cuota y formato Pisos
</commit_message>
<xml_diff>
--- a/backend/docs/ACT-AUT.xlsx
+++ b/backend/docs/ACT-AUT.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\coreui-free-react-admin-template-main\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\planosperu-app\backend\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB6A8CF-8DF5-490C-B7F7-D216B065AFC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C2CA4C-9A96-433D-AE77-933F527268A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{96D1BB80-F449-4442-8AAB-F71CF7F38B12}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7785" xr2:uid="{96D1BB80-F449-4442-8AAB-F71CF7F38B12}"/>
   </bookViews>
   <sheets>
     <sheet name="ACT-AUT" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Print_Area" localSheetId="0">'ACT-AUT'!$A$1:$H$71</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'ACT-AUT'!$A$1:$H$71</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -709,10 +709,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -804,27 +800,351 @@
     <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -838,348 +1158,28 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1844,9 +1844,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1884,7 +1884,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1990,7 +1990,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2132,7 +2132,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2150,7 +2150,7 @@
       <selection activeCell="B64" sqref="B64:E64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" customWidth="1"/>
@@ -2169,86 +2169,86 @@
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="140" t="s">
+      <c r="D4" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="140"/>
-      <c r="F4" s="140"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="141" t="s">
+      <c r="D5" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="141"/>
-      <c r="F5" s="141"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="142" t="s">
+      <c r="D6" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="142"/>
-      <c r="F6" s="142"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="143" t="s">
+      <c r="D7" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="143"/>
-      <c r="F7" s="143"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="144"/>
-      <c r="B8" s="144"/>
-      <c r="C8" s="144"/>
-      <c r="D8" s="144"/>
-      <c r="E8" s="144"/>
-      <c r="F8" s="144"/>
-      <c r="G8" s="144"/>
-      <c r="H8" s="144"/>
+      <c r="A8" s="45"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
     </row>
     <row r="9" spans="1:8" s="5" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="145" t="s">
+      <c r="B9" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="145"/>
-      <c r="D9" s="145"/>
-      <c r="E9" s="145"/>
-      <c r="F9" s="145"/>
-      <c r="G9" s="145"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:8" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="145"/>
-      <c r="C10" s="145"/>
-      <c r="D10" s="145"/>
-      <c r="E10" s="145"/>
-      <c r="F10" s="145"/>
-      <c r="G10" s="145"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="138" t="s">
+      <c r="B11" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="138"/>
-      <c r="D11" s="138"/>
-      <c r="E11" s="138"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
       <c r="F11" s="8" t="s">
         <v>12</v>
       </c>
@@ -2257,734 +2257,734 @@
     </row>
     <row r="12" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="138"/>
-      <c r="C12" s="138"/>
-      <c r="D12" s="138"/>
-      <c r="E12" s="138"/>
-      <c r="F12" s="138"/>
-      <c r="G12" s="138"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
-      <c r="B13" s="138"/>
-      <c r="C13" s="138"/>
-      <c r="D13" s="138"/>
-      <c r="E13" s="138"/>
-      <c r="F13" s="138"/>
-      <c r="G13" s="138"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="14" t="s">
+      <c r="B14" s="145"/>
+      <c r="C14" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="16" t="s">
+      <c r="D14" s="14"/>
+      <c r="E14" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="17"/>
+      <c r="G14" s="16"/>
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="138"/>
-      <c r="C15" s="138"/>
-      <c r="D15" s="138"/>
-      <c r="E15" s="138"/>
-      <c r="F15" s="14" t="s">
+      <c r="B15" s="49"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="17"/>
+      <c r="G15" s="16"/>
       <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
-      <c r="B16" s="139"/>
-      <c r="C16" s="139"/>
-      <c r="D16" s="139"/>
-      <c r="E16" s="139"/>
-      <c r="F16" s="14" t="s">
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="18"/>
+      <c r="G16" s="17"/>
       <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="138"/>
-      <c r="C17" s="138"/>
-      <c r="D17" s="19" t="s">
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="19">
         <f ca="1">TODAY()</f>
-        <v>45782</v>
-      </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
+        <v>45827</v>
+      </c>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
     </row>
     <row r="18" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="128"/>
-      <c r="C18" s="128"/>
-      <c r="D18" s="128"/>
-      <c r="E18" s="128"/>
-      <c r="F18" s="128"/>
-      <c r="G18" s="128"/>
-      <c r="H18" s="21"/>
-    </row>
-    <row r="19" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="129" t="s">
+      <c r="A18" s="20"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="20"/>
+    </row>
+    <row r="19" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="21"/>
+      <c r="B19" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="130"/>
-      <c r="D19" s="131"/>
-      <c r="E19" s="132"/>
-      <c r="F19" s="132"/>
-      <c r="G19" s="132"/>
-      <c r="H19" s="23"/>
-    </row>
-    <row r="20" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="53"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="55"/>
+      <c r="H19" s="22"/>
+    </row>
+    <row r="20" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
-      <c r="B20" s="133" t="s">
+      <c r="B20" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="134"/>
-      <c r="D20" s="135"/>
-      <c r="E20" s="136" t="s">
+      <c r="C20" s="57"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="136"/>
-      <c r="G20" s="137"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="60"/>
       <c r="H20" s="10"/>
     </row>
-    <row r="21" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
-      <c r="B21" s="76" t="s">
+      <c r="B21" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="77"/>
-      <c r="D21" s="78"/>
-      <c r="E21" s="77" t="s">
+      <c r="C21" s="47"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="F21" s="77"/>
-      <c r="G21" s="78"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="48"/>
       <c r="H21" s="10"/>
     </row>
-    <row r="22" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
-      <c r="B22" s="66" t="s">
+      <c r="B22" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="67"/>
-      <c r="D22" s="67"/>
-      <c r="E22" s="126"/>
-      <c r="F22" s="126"/>
-      <c r="G22" s="127"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="63"/>
+      <c r="F22" s="63"/>
+      <c r="G22" s="64"/>
       <c r="H22" s="10"/>
     </row>
-    <row r="23" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
-      <c r="B23" s="76" t="s">
+      <c r="B23" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="77"/>
-      <c r="D23" s="78"/>
-      <c r="E23" s="76" t="s">
+      <c r="C23" s="47"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="77"/>
-      <c r="G23" s="78"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="48"/>
       <c r="H23" s="10"/>
     </row>
-    <row r="24" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
-      <c r="B24" s="76" t="s">
+      <c r="B24" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="77"/>
-      <c r="D24" s="78"/>
-      <c r="E24" s="76" t="s">
+      <c r="C24" s="47"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="F24" s="77"/>
-      <c r="G24" s="78"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="48"/>
       <c r="H24" s="10"/>
     </row>
-    <row r="25" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="25"/>
-      <c r="B25" s="76" t="s">
+    <row r="25" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="24"/>
+      <c r="B25" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="77"/>
-      <c r="D25" s="78"/>
-      <c r="E25" s="76" t="s">
+      <c r="C25" s="47"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="77"/>
-      <c r="G25" s="78"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="48"/>
       <c r="H25" s="10"/>
     </row>
-    <row r="26" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
-      <c r="B26" s="76" t="s">
+    <row r="26" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="25"/>
+      <c r="B26" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="78"/>
-      <c r="E26" s="76" t="s">
+      <c r="C26" s="47"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="F26" s="77"/>
-      <c r="G26" s="78"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="48"/>
       <c r="H26" s="10"/>
     </row>
-    <row r="27" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
-      <c r="B27" s="60" t="s">
+    <row r="27" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="25"/>
+      <c r="B27" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="61"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="76" t="s">
+      <c r="C27" s="69"/>
+      <c r="D27" s="70"/>
+      <c r="E27" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="77"/>
-      <c r="G27" s="78"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="48"/>
       <c r="H27" s="10"/>
     </row>
-    <row r="28" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
-      <c r="B28" s="112" t="s">
+    <row r="28" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="25"/>
+      <c r="B28" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="113"/>
-      <c r="D28" s="114"/>
-      <c r="E28" s="115" t="s">
+      <c r="C28" s="72"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="F28" s="116"/>
-      <c r="G28" s="117"/>
+      <c r="F28" s="75"/>
+      <c r="G28" s="76"/>
       <c r="H28" s="10"/>
     </row>
-    <row r="29" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="26"/>
-      <c r="B29" s="66" t="s">
+    <row r="29" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="25"/>
+      <c r="B29" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="67"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="118"/>
-      <c r="F29" s="118"/>
-      <c r="G29" s="119"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="77"/>
+      <c r="F29" s="77"/>
+      <c r="G29" s="78"/>
       <c r="H29" s="10"/>
     </row>
-    <row r="30" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
-      <c r="B30" s="120" t="s">
+    <row r="30" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="26"/>
+      <c r="B30" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="121"/>
-      <c r="D30" s="122"/>
-      <c r="E30" s="123" t="s">
+      <c r="C30" s="80"/>
+      <c r="D30" s="81"/>
+      <c r="E30" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="F30" s="124"/>
-      <c r="G30" s="125"/>
+      <c r="F30" s="83"/>
+      <c r="G30" s="84"/>
       <c r="H30" s="10"/>
     </row>
-    <row r="31" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="27"/>
-      <c r="B31" s="97" t="s">
+    <row r="31" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="26"/>
+      <c r="B31" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="98"/>
-      <c r="D31" s="99"/>
-      <c r="E31" s="28" t="s">
+      <c r="C31" s="66"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F31" s="29"/>
-      <c r="G31" s="30"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="29"/>
       <c r="H31" s="10"/>
     </row>
-    <row r="32" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
-      <c r="B32" s="106" t="s">
+    <row r="32" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="30"/>
+      <c r="B32" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="107"/>
-      <c r="D32" s="108"/>
-      <c r="E32" s="28" t="s">
+      <c r="C32" s="86"/>
+      <c r="D32" s="87"/>
+      <c r="E32" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="F32" s="29"/>
-      <c r="G32" s="30"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="29"/>
       <c r="H32" s="10"/>
     </row>
-    <row r="33" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
-      <c r="B33" s="106"/>
-      <c r="C33" s="107"/>
-      <c r="D33" s="108"/>
-      <c r="E33" s="60" t="s">
+      <c r="B33" s="85"/>
+      <c r="C33" s="86"/>
+      <c r="D33" s="87"/>
+      <c r="E33" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="F33" s="61"/>
-      <c r="G33" s="62"/>
+      <c r="F33" s="69"/>
+      <c r="G33" s="70"/>
       <c r="H33" s="10"/>
     </row>
-    <row r="34" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
-      <c r="B34" s="60" t="s">
+      <c r="B34" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="61"/>
-      <c r="D34" s="62"/>
-      <c r="E34" s="60" t="s">
+      <c r="C34" s="69"/>
+      <c r="D34" s="70"/>
+      <c r="E34" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="F34" s="61"/>
-      <c r="G34" s="62"/>
+      <c r="F34" s="69"/>
+      <c r="G34" s="70"/>
       <c r="H34" s="10"/>
     </row>
-    <row r="35" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
-      <c r="B35" s="109" t="s">
+      <c r="B35" s="88" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="110"/>
-      <c r="D35" s="111"/>
-      <c r="E35" s="60" t="s">
+      <c r="C35" s="89"/>
+      <c r="D35" s="90"/>
+      <c r="E35" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="F35" s="61"/>
-      <c r="G35" s="62"/>
+      <c r="F35" s="69"/>
+      <c r="G35" s="70"/>
       <c r="H35" s="10"/>
     </row>
-    <row r="36" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
-      <c r="B36" s="109"/>
-      <c r="C36" s="110"/>
-      <c r="D36" s="111"/>
-      <c r="E36" s="82" t="s">
+      <c r="B36" s="88"/>
+      <c r="C36" s="89"/>
+      <c r="D36" s="90"/>
+      <c r="E36" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="F36" s="61"/>
-      <c r="G36" s="62"/>
+      <c r="F36" s="69"/>
+      <c r="G36" s="70"/>
       <c r="H36" s="10"/>
     </row>
-    <row r="37" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
-      <c r="B37" s="94" t="s">
+      <c r="B37" s="95" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="95"/>
-      <c r="D37" s="96"/>
-      <c r="E37" s="85" t="s">
+      <c r="C37" s="96"/>
+      <c r="D37" s="97"/>
+      <c r="E37" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="F37" s="86"/>
-      <c r="G37" s="87"/>
+      <c r="F37" s="99"/>
+      <c r="G37" s="100"/>
       <c r="H37" s="10"/>
     </row>
-    <row r="38" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
-      <c r="B38" s="97" t="s">
+      <c r="B38" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="C38" s="98"/>
-      <c r="D38" s="99"/>
-      <c r="E38" s="85"/>
-      <c r="F38" s="86"/>
-      <c r="G38" s="87"/>
+      <c r="C38" s="66"/>
+      <c r="D38" s="67"/>
+      <c r="E38" s="98"/>
+      <c r="F38" s="99"/>
+      <c r="G38" s="100"/>
       <c r="H38" s="10"/>
     </row>
-    <row r="39" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
-      <c r="B39" s="73" t="s">
+      <c r="B39" s="101" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="74"/>
-      <c r="D39" s="75"/>
-      <c r="E39" s="100" t="s">
+      <c r="C39" s="102"/>
+      <c r="D39" s="103"/>
+      <c r="E39" s="104" t="s">
         <v>57</v>
       </c>
-      <c r="F39" s="101"/>
-      <c r="G39" s="102"/>
+      <c r="F39" s="105"/>
+      <c r="G39" s="106"/>
       <c r="H39" s="10"/>
     </row>
-    <row r="40" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
-      <c r="B40" s="73"/>
-      <c r="C40" s="74"/>
-      <c r="D40" s="75"/>
-      <c r="E40" s="103" t="s">
+      <c r="B40" s="101"/>
+      <c r="C40" s="102"/>
+      <c r="D40" s="103"/>
+      <c r="E40" s="107" t="s">
         <v>58</v>
       </c>
-      <c r="F40" s="104"/>
-      <c r="G40" s="105"/>
+      <c r="F40" s="108"/>
+      <c r="G40" s="109"/>
       <c r="H40" s="10"/>
     </row>
-    <row r="41" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
-      <c r="B41" s="60" t="s">
+      <c r="B41" s="68" t="s">
         <v>59</v>
       </c>
-      <c r="C41" s="61"/>
-      <c r="D41" s="62"/>
-      <c r="E41" s="85" t="s">
+      <c r="C41" s="69"/>
+      <c r="D41" s="70"/>
+      <c r="E41" s="98" t="s">
         <v>60</v>
       </c>
-      <c r="F41" s="86"/>
-      <c r="G41" s="87"/>
+      <c r="F41" s="99"/>
+      <c r="G41" s="100"/>
       <c r="H41" s="10"/>
     </row>
-    <row r="42" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
-      <c r="B42" s="60" t="s">
+      <c r="B42" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="C42" s="61"/>
-      <c r="D42" s="62"/>
-      <c r="E42" s="85"/>
-      <c r="F42" s="86"/>
-      <c r="G42" s="87"/>
+      <c r="C42" s="69"/>
+      <c r="D42" s="70"/>
+      <c r="E42" s="98"/>
+      <c r="F42" s="99"/>
+      <c r="G42" s="100"/>
       <c r="H42" s="10"/>
     </row>
-    <row r="43" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
-      <c r="B43" s="60" t="s">
+      <c r="B43" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="C43" s="61"/>
-      <c r="D43" s="62"/>
-      <c r="E43" s="88" t="s">
+      <c r="C43" s="69"/>
+      <c r="D43" s="70"/>
+      <c r="E43" s="110" t="s">
         <v>63</v>
       </c>
-      <c r="F43" s="89"/>
-      <c r="G43" s="90"/>
+      <c r="F43" s="111"/>
+      <c r="G43" s="112"/>
       <c r="H43" s="10"/>
     </row>
-    <row r="44" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
-      <c r="B44" s="60" t="s">
+      <c r="B44" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="C44" s="61"/>
-      <c r="D44" s="62"/>
-      <c r="E44" s="91"/>
-      <c r="F44" s="92"/>
-      <c r="G44" s="93"/>
+      <c r="C44" s="69"/>
+      <c r="D44" s="70"/>
+      <c r="E44" s="92"/>
+      <c r="F44" s="93"/>
+      <c r="G44" s="94"/>
       <c r="H44" s="10"/>
     </row>
-    <row r="45" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
-      <c r="B45" s="60" t="s">
+      <c r="B45" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="C45" s="61"/>
-      <c r="D45" s="62"/>
-      <c r="E45" s="63"/>
-      <c r="F45" s="64"/>
-      <c r="G45" s="65"/>
+      <c r="C45" s="69"/>
+      <c r="D45" s="70"/>
+      <c r="E45" s="114"/>
+      <c r="F45" s="115"/>
+      <c r="G45" s="116"/>
       <c r="H45" s="10"/>
     </row>
-    <row r="46" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="66" t="s">
+    <row r="46" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="C46" s="67"/>
-      <c r="D46" s="67"/>
-      <c r="E46" s="68"/>
-      <c r="F46" s="68"/>
-      <c r="G46" s="69"/>
+      <c r="C46" s="62"/>
+      <c r="D46" s="62"/>
+      <c r="E46" s="117"/>
+      <c r="F46" s="117"/>
+      <c r="G46" s="118"/>
       <c r="H46" s="10"/>
     </row>
-    <row r="47" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
-      <c r="B47" s="70" t="s">
+      <c r="B47" s="119" t="s">
         <v>67</v>
       </c>
-      <c r="C47" s="71"/>
-      <c r="D47" s="72"/>
-      <c r="E47" s="76" t="s">
+      <c r="C47" s="120"/>
+      <c r="D47" s="121"/>
+      <c r="E47" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="F47" s="77"/>
-      <c r="G47" s="78"/>
+      <c r="F47" s="47"/>
+      <c r="G47" s="48"/>
       <c r="H47" s="10"/>
     </row>
-    <row r="48" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
-      <c r="B48" s="73"/>
-      <c r="C48" s="74"/>
-      <c r="D48" s="75"/>
-      <c r="E48" s="79" t="s">
+      <c r="B48" s="101"/>
+      <c r="C48" s="102"/>
+      <c r="D48" s="103"/>
+      <c r="E48" s="122" t="s">
         <v>69</v>
       </c>
-      <c r="F48" s="80"/>
-      <c r="G48" s="81"/>
+      <c r="F48" s="123"/>
+      <c r="G48" s="124"/>
       <c r="H48" s="10"/>
     </row>
-    <row r="49" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
-      <c r="B49" s="73"/>
-      <c r="C49" s="74"/>
-      <c r="D49" s="75"/>
-      <c r="E49" s="82" t="s">
+      <c r="B49" s="101"/>
+      <c r="C49" s="102"/>
+      <c r="D49" s="103"/>
+      <c r="E49" s="91" t="s">
         <v>70</v>
       </c>
-      <c r="F49" s="83"/>
-      <c r="G49" s="84"/>
+      <c r="F49" s="125"/>
+      <c r="G49" s="126"/>
       <c r="H49" s="10"/>
     </row>
-    <row r="50" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>
-      <c r="B50" s="51" t="s">
+      <c r="B50" s="127" t="s">
         <v>71</v>
       </c>
-      <c r="C50" s="52"/>
-      <c r="D50" s="53"/>
-      <c r="E50" s="54"/>
-      <c r="F50" s="55"/>
-      <c r="G50" s="56"/>
+      <c r="C50" s="128"/>
+      <c r="D50" s="129"/>
+      <c r="E50" s="130"/>
+      <c r="F50" s="131"/>
+      <c r="G50" s="132"/>
       <c r="H50" s="10"/>
     </row>
-    <row r="51" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
-      <c r="B51" s="57"/>
-      <c r="C51" s="57"/>
-      <c r="D51" s="57"/>
-      <c r="E51" s="57"/>
-      <c r="F51" s="57"/>
-      <c r="G51" s="57"/>
+      <c r="B51" s="133"/>
+      <c r="C51" s="133"/>
+      <c r="D51" s="133"/>
+      <c r="E51" s="133"/>
+      <c r="F51" s="133"/>
+      <c r="G51" s="133"/>
       <c r="H51" s="10"/>
     </row>
-    <row r="52" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
-      <c r="B52" s="32" t="s">
+      <c r="B52" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C52" s="58"/>
-      <c r="D52" s="58"/>
-      <c r="E52" s="58"/>
-      <c r="F52" s="58"/>
-      <c r="G52" s="58"/>
+      <c r="C52" s="134"/>
+      <c r="D52" s="134"/>
+      <c r="E52" s="134"/>
+      <c r="F52" s="134"/>
+      <c r="G52" s="134"/>
       <c r="H52" s="10"/>
     </row>
-    <row r="53" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
-      <c r="B53" s="59"/>
-      <c r="C53" s="59"/>
-      <c r="D53" s="59"/>
-      <c r="E53" s="59"/>
-      <c r="F53" s="59"/>
-      <c r="G53" s="59"/>
+      <c r="B53" s="113"/>
+      <c r="C53" s="113"/>
+      <c r="D53" s="113"/>
+      <c r="E53" s="113"/>
+      <c r="F53" s="113"/>
+      <c r="G53" s="113"/>
       <c r="H53" s="10"/>
     </row>
-    <row r="54" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
-      <c r="B54" s="59"/>
-      <c r="C54" s="59"/>
-      <c r="D54" s="59"/>
-      <c r="E54" s="59"/>
-      <c r="F54" s="59"/>
-      <c r="G54" s="59"/>
+      <c r="B54" s="113"/>
+      <c r="C54" s="113"/>
+      <c r="D54" s="113"/>
+      <c r="E54" s="113"/>
+      <c r="F54" s="113"/>
+      <c r="G54" s="113"/>
       <c r="H54" s="10"/>
     </row>
-    <row r="55" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
-      <c r="B55" s="47"/>
-      <c r="C55" s="47"/>
-      <c r="D55" s="47"/>
-      <c r="E55" s="47"/>
-      <c r="F55" s="47"/>
-      <c r="G55" s="47"/>
+      <c r="B55" s="135"/>
+      <c r="C55" s="135"/>
+      <c r="D55" s="135"/>
+      <c r="E55" s="135"/>
+      <c r="F55" s="135"/>
+      <c r="G55" s="135"/>
       <c r="H55" s="10"/>
     </row>
-    <row r="56" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="22"/>
-      <c r="B56" s="43" t="s">
+    <row r="56" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="21"/>
+      <c r="B56" s="136" t="s">
         <v>73</v>
       </c>
-      <c r="C56" s="43"/>
-      <c r="D56" s="43"/>
-      <c r="E56" s="43"/>
-      <c r="F56" s="43"/>
-      <c r="G56" s="43"/>
-      <c r="H56" s="23"/>
-    </row>
-    <row r="57" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="23"/>
-      <c r="B57" s="48" t="s">
+      <c r="C56" s="136"/>
+      <c r="D56" s="136"/>
+      <c r="E56" s="136"/>
+      <c r="F56" s="136"/>
+      <c r="G56" s="136"/>
+      <c r="H56" s="22"/>
+    </row>
+    <row r="57" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="22"/>
+      <c r="B57" s="137" t="s">
         <v>74</v>
       </c>
-      <c r="C57" s="48"/>
-      <c r="D57" s="33">
+      <c r="C57" s="137"/>
+      <c r="D57" s="32">
         <v>7</v>
       </c>
-      <c r="E57" s="21" t="s">
+      <c r="E57" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="F57" s="21"/>
-      <c r="G57" s="21"/>
-      <c r="H57" s="23"/>
-    </row>
-    <row r="58" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="22"/>
-      <c r="B58" s="43" t="s">
+      <c r="F57" s="20"/>
+      <c r="G57" s="20"/>
+      <c r="H57" s="22"/>
+    </row>
+    <row r="58" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="21"/>
+      <c r="B58" s="136" t="s">
         <v>76</v>
       </c>
-      <c r="C58" s="43"/>
-      <c r="D58" s="43"/>
-      <c r="E58" s="43"/>
-      <c r="F58" s="43"/>
-      <c r="G58" s="43"/>
-      <c r="H58" s="23"/>
-    </row>
-    <row r="59" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="23"/>
-      <c r="B59" s="49" t="s">
+      <c r="C58" s="136"/>
+      <c r="D58" s="136"/>
+      <c r="E58" s="136"/>
+      <c r="F58" s="136"/>
+      <c r="G58" s="136"/>
+      <c r="H58" s="22"/>
+    </row>
+    <row r="59" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="22"/>
+      <c r="B59" s="138" t="s">
         <v>77</v>
       </c>
-      <c r="C59" s="49"/>
-      <c r="D59" s="34">
+      <c r="C59" s="138"/>
+      <c r="D59" s="33">
         <f>SUM(C61:C61)</f>
         <v>0</v>
       </c>
-      <c r="E59" s="50" t="s">
+      <c r="E59" s="139" t="s">
         <v>78</v>
       </c>
-      <c r="F59" s="50"/>
-      <c r="G59" s="21"/>
-      <c r="H59" s="23"/>
-    </row>
-    <row r="60" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="22"/>
-      <c r="B60" s="43" t="s">
+      <c r="F59" s="139"/>
+      <c r="G59" s="20"/>
+      <c r="H59" s="22"/>
+    </row>
+    <row r="60" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="21"/>
+      <c r="B60" s="136" t="s">
         <v>79</v>
       </c>
-      <c r="C60" s="43"/>
-      <c r="D60" s="43"/>
-      <c r="E60" s="43"/>
-      <c r="F60" s="43"/>
-      <c r="G60" s="43"/>
-      <c r="H60" s="23"/>
-    </row>
-    <row r="61" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="23"/>
-      <c r="B61" s="35" t="s">
+      <c r="C60" s="136"/>
+      <c r="D60" s="136"/>
+      <c r="E60" s="136"/>
+      <c r="F60" s="136"/>
+      <c r="G60" s="136"/>
+      <c r="H60" s="22"/>
+    </row>
+    <row r="61" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="22"/>
+      <c r="B61" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="C61" s="36"/>
-      <c r="D61" s="44" t="s">
+      <c r="C61" s="35"/>
+      <c r="D61" s="140" t="s">
         <v>81</v>
       </c>
-      <c r="E61" s="44"/>
-      <c r="F61" s="44"/>
-      <c r="G61" s="37">
+      <c r="E61" s="140"/>
+      <c r="F61" s="140"/>
+      <c r="G61" s="36">
         <f ca="1">E17</f>
-        <v>45782</v>
-      </c>
-      <c r="H61" s="23"/>
-    </row>
-    <row r="62" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+        <v>45827</v>
+      </c>
+      <c r="H61" s="22"/>
+    </row>
+    <row r="62" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
-      <c r="B62" s="45" t="s">
+      <c r="B62" s="141" t="s">
         <v>82</v>
       </c>
-      <c r="C62" s="45"/>
-      <c r="D62" s="45"/>
-      <c r="E62" s="45"/>
-      <c r="F62" s="45"/>
-      <c r="G62" s="45"/>
-      <c r="H62" s="38"/>
-    </row>
-    <row r="63" spans="1:8" s="24" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="39" t="s">
+      <c r="C62" s="141"/>
+      <c r="D62" s="141"/>
+      <c r="E62" s="141"/>
+      <c r="F62" s="141"/>
+      <c r="G62" s="141"/>
+      <c r="H62" s="37"/>
+    </row>
+    <row r="63" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="B63" s="46" t="s">
+      <c r="B63" s="142" t="s">
         <v>84</v>
       </c>
-      <c r="C63" s="46"/>
-      <c r="D63" s="46"/>
-      <c r="E63" s="46"/>
-      <c r="F63" s="46"/>
-      <c r="G63" s="46"/>
+      <c r="C63" s="142"/>
+      <c r="D63" s="142"/>
+      <c r="E63" s="142"/>
+      <c r="F63" s="142"/>
+      <c r="G63" s="142"/>
     </row>
     <row r="64" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="42" t="s">
+      <c r="B64" s="143" t="s">
         <v>85</v>
       </c>
-      <c r="C64" s="42"/>
-      <c r="D64" s="42"/>
-      <c r="E64" s="42"/>
-      <c r="F64" s="42" t="s">
+      <c r="C64" s="143"/>
+      <c r="D64" s="143"/>
+      <c r="E64" s="143"/>
+      <c r="F64" s="143" t="s">
         <v>86</v>
       </c>
-      <c r="G64" s="42"/>
-      <c r="H64" s="42"/>
+      <c r="G64" s="143"/>
+      <c r="H64" s="143"/>
     </row>
     <row r="65" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="41" t="s">
+      <c r="B65" s="144" t="s">
         <v>87</v>
       </c>
-      <c r="C65" s="41"/>
-      <c r="D65" s="41"/>
-      <c r="E65" s="41"/>
-      <c r="F65" s="42" t="s">
+      <c r="C65" s="144"/>
+      <c r="D65" s="144"/>
+      <c r="E65" s="144"/>
+      <c r="F65" s="143" t="s">
         <v>88</v>
       </c>
-      <c r="G65" s="42"/>
-      <c r="H65" s="42"/>
+      <c r="G65" s="143"/>
+      <c r="H65" s="143"/>
     </row>
     <row r="66" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="41" t="s">
+      <c r="B66" s="144" t="s">
         <v>89</v>
       </c>
-      <c r="C66" s="41"/>
-      <c r="D66" s="41"/>
-      <c r="E66" s="41"/>
-      <c r="F66" s="42" t="s">
+      <c r="C66" s="144"/>
+      <c r="D66" s="144"/>
+      <c r="E66" s="144"/>
+      <c r="F66" s="143" t="s">
         <v>90</v>
       </c>
-      <c r="G66" s="42"/>
-      <c r="H66" s="42"/>
+      <c r="G66" s="143"/>
+      <c r="H66" s="143"/>
     </row>
     <row r="67" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="42" t="s">
+      <c r="B67" s="143" t="s">
         <v>91</v>
       </c>
-      <c r="C67" s="42"/>
-      <c r="D67" s="42"/>
-      <c r="E67" s="42"/>
-      <c r="F67" s="42"/>
-      <c r="G67" s="42"/>
+      <c r="C67" s="143"/>
+      <c r="D67" s="143"/>
+      <c r="E67" s="143"/>
+      <c r="F67" s="143"/>
+      <c r="G67" s="143"/>
     </row>
     <row r="68" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="40"/>
-      <c r="C68" s="40"/>
-      <c r="D68" s="40"/>
-      <c r="E68" s="40"/>
-      <c r="F68" s="40"/>
-      <c r="G68" s="40"/>
-      <c r="H68" s="40"/>
+      <c r="B68" s="39"/>
+      <c r="C68" s="39"/>
+      <c r="D68" s="39"/>
+      <c r="E68" s="39"/>
+      <c r="F68" s="39"/>
+      <c r="G68" s="39"/>
+      <c r="H68" s="39"/>
     </row>
     <row r="71" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="72" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3005,12 +3005,75 @@
     <protectedRange algorithmName="SHA-512" hashValue="1IwEtpPovyRjspz9ti3J5udl070IPZ9gDlGmM3ZH/lFyQlLVVL2qbaMds7kHvZZkPq7VvowLV2MqpNnf8owpjQ==" saltValue="SwYyjj//I75seGLqQP0hyQ==" spinCount="100000" sqref="E37:G38 E39" name="Rango2_2"/>
   </protectedRanges>
   <mergeCells count="88">
-    <mergeCell ref="B9:G10"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="B66:E66"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="B62:G62"/>
+    <mergeCell ref="B63:G63"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="B56:G56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="B47:D49"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="C52:G52"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:G38"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B39:D40"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="E41:G42"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="B32:D33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="B35:D36"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:G24"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="E21:G21"/>
     <mergeCell ref="B11:E11"/>
@@ -3024,75 +3087,12 @@
     <mergeCell ref="E19:G19"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="E20:G20"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="B32:D33"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="B35:D36"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E37:G38"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B39:D40"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="E41:G42"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="B54:G54"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="B46:G46"/>
-    <mergeCell ref="B47:D49"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="C52:G52"/>
-    <mergeCell ref="B53:G53"/>
-    <mergeCell ref="B55:G55"/>
-    <mergeCell ref="B56:G56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:G58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="B62:G62"/>
-    <mergeCell ref="B63:G63"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="B66:E66"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="B9:G10"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="A8:H8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D7" r:id="rId1" xr:uid="{06F8AEE0-B467-46CC-BA80-3945E484B37D}"/>

</xml_diff>

<commit_message>
feat: agregado cuotas a cotizacion
</commit_message>
<xml_diff>
--- a/backend/docs/ACT-AUT.xlsx
+++ b/backend/docs/ACT-AUT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\planosperu-app\backend\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C2CA4C-9A96-433D-AE77-933F527268A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FF0D8D-8479-4346-AB6D-48E419609CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7785" xr2:uid="{96D1BB80-F449-4442-8AAB-F71CF7F38B12}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{96D1BB80-F449-4442-8AAB-F71CF7F38B12}"/>
   </bookViews>
   <sheets>
     <sheet name="ACT-AUT" sheetId="2" r:id="rId1"/>
@@ -281,9 +281,6 @@
     <t>5.-MODO DE CANCELACIÓN:</t>
   </si>
   <si>
-    <t xml:space="preserve">   S/   </t>
-  </si>
-  <si>
     <t xml:space="preserve">A la Aprobación de la Presente Proforma  </t>
   </si>
   <si>
@@ -315,6 +312,9 @@
   </si>
   <si>
     <t>Ing. Sanitario José Francisco Javier Zela Steban CIP: 130333</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuota 1 S/  </t>
   </si>
 </sst>
 </file>
@@ -800,77 +800,62 @@
     <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
@@ -879,119 +864,103 @@
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -1022,16 +991,16 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1061,122 +1030,153 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2169,86 +2169,86 @@
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="141" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
+      <c r="E4" s="141"/>
+      <c r="F4" s="141"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="142" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
+      <c r="E5" s="142"/>
+      <c r="F5" s="142"/>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="43" t="s">
+      <c r="D6" s="143" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
+      <c r="E6" s="143"/>
+      <c r="F6" s="143"/>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="144" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
+      <c r="E7" s="144"/>
+      <c r="F7" s="144"/>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
+      <c r="A8" s="145"/>
+      <c r="B8" s="145"/>
+      <c r="C8" s="145"/>
+      <c r="D8" s="145"/>
+      <c r="E8" s="145"/>
+      <c r="F8" s="145"/>
+      <c r="G8" s="145"/>
+      <c r="H8" s="145"/>
     </row>
     <row r="9" spans="1:8" s="5" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="140" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
+      <c r="C9" s="140"/>
+      <c r="D9" s="140"/>
+      <c r="E9" s="140"/>
+      <c r="F9" s="140"/>
+      <c r="G9" s="140"/>
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:8" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="40"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
+      <c r="B10" s="140"/>
+      <c r="C10" s="140"/>
+      <c r="D10" s="140"/>
+      <c r="E10" s="140"/>
+      <c r="F10" s="140"/>
+      <c r="G10" s="140"/>
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="128" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
+      <c r="C11" s="128"/>
+      <c r="D11" s="128"/>
+      <c r="E11" s="128"/>
       <c r="F11" s="8" t="s">
         <v>12</v>
       </c>
@@ -2257,29 +2257,29 @@
     </row>
     <row r="12" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
+      <c r="B12" s="128"/>
+      <c r="C12" s="128"/>
+      <c r="D12" s="128"/>
+      <c r="E12" s="128"/>
+      <c r="F12" s="128"/>
+      <c r="G12" s="128"/>
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
+      <c r="B13" s="128"/>
+      <c r="C13" s="128"/>
+      <c r="D13" s="128"/>
+      <c r="E13" s="128"/>
+      <c r="F13" s="128"/>
+      <c r="G13" s="128"/>
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="145"/>
+      <c r="B14" s="40"/>
       <c r="C14" s="13" t="s">
         <v>14</v>
       </c>
@@ -2297,10 +2297,10 @@
       <c r="A15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="49"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
+      <c r="B15" s="128"/>
+      <c r="C15" s="128"/>
+      <c r="D15" s="128"/>
+      <c r="E15" s="128"/>
       <c r="F15" s="13" t="s">
         <v>18</v>
       </c>
@@ -2309,10 +2309,10 @@
     </row>
     <row r="16" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
-      <c r="B16" s="50"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
+      <c r="B16" s="129"/>
+      <c r="C16" s="129"/>
+      <c r="D16" s="129"/>
+      <c r="E16" s="129"/>
       <c r="F16" s="13" t="s">
         <v>19</v>
       </c>
@@ -2323,14 +2323,14 @@
       <c r="A17" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
+      <c r="B17" s="128"/>
+      <c r="C17" s="128"/>
       <c r="D17" s="18" t="s">
         <v>21</v>
       </c>
       <c r="E17" s="19">
         <f ca="1">TODAY()</f>
-        <v>45827</v>
+        <v>45838</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
@@ -2338,183 +2338,183 @@
     </row>
     <row r="18" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
+      <c r="B18" s="130"/>
+      <c r="C18" s="130"/>
+      <c r="D18" s="130"/>
+      <c r="E18" s="130"/>
+      <c r="F18" s="130"/>
+      <c r="G18" s="130"/>
       <c r="H18" s="20"/>
     </row>
     <row r="19" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
-      <c r="B19" s="52" t="s">
+      <c r="B19" s="131" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="53"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="55"/>
+      <c r="C19" s="132"/>
+      <c r="D19" s="133"/>
+      <c r="E19" s="134"/>
+      <c r="F19" s="134"/>
+      <c r="G19" s="134"/>
       <c r="H19" s="22"/>
     </row>
     <row r="20" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
-      <c r="B20" s="56" t="s">
+      <c r="B20" s="135" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="57"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="59" t="s">
+      <c r="C20" s="136"/>
+      <c r="D20" s="137"/>
+      <c r="E20" s="138" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="59"/>
-      <c r="G20" s="60"/>
+      <c r="F20" s="138"/>
+      <c r="G20" s="139"/>
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="47"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="47" t="s">
+      <c r="C21" s="69"/>
+      <c r="D21" s="70"/>
+      <c r="E21" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="F21" s="47"/>
-      <c r="G21" s="48"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="70"/>
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
-      <c r="B22" s="61" t="s">
+      <c r="B22" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="63"/>
-      <c r="F22" s="63"/>
-      <c r="G22" s="64"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="126"/>
+      <c r="F22" s="126"/>
+      <c r="G22" s="127"/>
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
-      <c r="B23" s="46" t="s">
+      <c r="B23" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="47"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="46" t="s">
+      <c r="C23" s="69"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="47"/>
-      <c r="G23" s="48"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="70"/>
       <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="47"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="46" t="s">
+      <c r="C24" s="69"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="F24" s="47"/>
-      <c r="G24" s="48"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="70"/>
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="24"/>
-      <c r="B25" s="46" t="s">
+      <c r="B25" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="47"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="46" t="s">
+      <c r="C25" s="69"/>
+      <c r="D25" s="70"/>
+      <c r="E25" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="47"/>
-      <c r="G25" s="48"/>
+      <c r="F25" s="69"/>
+      <c r="G25" s="70"/>
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="25"/>
-      <c r="B26" s="46" t="s">
+      <c r="B26" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="47"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="46" t="s">
+      <c r="C26" s="69"/>
+      <c r="D26" s="70"/>
+      <c r="E26" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="F26" s="47"/>
-      <c r="G26" s="48"/>
+      <c r="F26" s="69"/>
+      <c r="G26" s="70"/>
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="25"/>
-      <c r="B27" s="68" t="s">
+      <c r="B27" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="69"/>
-      <c r="D27" s="70"/>
-      <c r="E27" s="46" t="s">
+      <c r="C27" s="53"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="47"/>
-      <c r="G27" s="48"/>
+      <c r="F27" s="69"/>
+      <c r="G27" s="70"/>
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="25"/>
-      <c r="B28" s="71" t="s">
+      <c r="B28" s="112" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="72"/>
-      <c r="D28" s="73"/>
-      <c r="E28" s="74" t="s">
+      <c r="C28" s="113"/>
+      <c r="D28" s="114"/>
+      <c r="E28" s="115" t="s">
         <v>39</v>
       </c>
-      <c r="F28" s="75"/>
-      <c r="G28" s="76"/>
+      <c r="F28" s="116"/>
+      <c r="G28" s="117"/>
       <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="25"/>
-      <c r="B29" s="61" t="s">
+      <c r="B29" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="62"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="77"/>
-      <c r="F29" s="77"/>
-      <c r="G29" s="78"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="118"/>
+      <c r="F29" s="118"/>
+      <c r="G29" s="119"/>
       <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="26"/>
-      <c r="B30" s="79" t="s">
+      <c r="B30" s="120" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="80"/>
-      <c r="D30" s="81"/>
-      <c r="E30" s="82" t="s">
+      <c r="C30" s="121"/>
+      <c r="D30" s="122"/>
+      <c r="E30" s="123" t="s">
         <v>42</v>
       </c>
-      <c r="F30" s="83"/>
-      <c r="G30" s="84"/>
+      <c r="F30" s="124"/>
+      <c r="G30" s="125"/>
       <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="26"/>
-      <c r="B31" s="65" t="s">
+      <c r="B31" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="66"/>
-      <c r="D31" s="67"/>
+      <c r="C31" s="95"/>
+      <c r="D31" s="96"/>
       <c r="E31" s="27" t="s">
         <v>44</v>
       </c>
@@ -2524,11 +2524,11 @@
     </row>
     <row r="32" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="30"/>
-      <c r="B32" s="85" t="s">
+      <c r="B32" s="106" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="86"/>
-      <c r="D32" s="87"/>
+      <c r="C32" s="107"/>
+      <c r="D32" s="108"/>
       <c r="E32" s="27" t="s">
         <v>46</v>
       </c>
@@ -2538,241 +2538,241 @@
     </row>
     <row r="33" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
-      <c r="B33" s="85"/>
-      <c r="C33" s="86"/>
-      <c r="D33" s="87"/>
-      <c r="E33" s="68" t="s">
+      <c r="B33" s="106"/>
+      <c r="C33" s="107"/>
+      <c r="D33" s="108"/>
+      <c r="E33" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="F33" s="69"/>
-      <c r="G33" s="70"/>
+      <c r="F33" s="53"/>
+      <c r="G33" s="54"/>
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
-      <c r="B34" s="68" t="s">
+      <c r="B34" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="69"/>
-      <c r="D34" s="70"/>
-      <c r="E34" s="68" t="s">
+      <c r="C34" s="53"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="F34" s="69"/>
-      <c r="G34" s="70"/>
+      <c r="F34" s="53"/>
+      <c r="G34" s="54"/>
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
-      <c r="B35" s="88" t="s">
+      <c r="B35" s="109" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="89"/>
-      <c r="D35" s="90"/>
-      <c r="E35" s="68" t="s">
+      <c r="C35" s="110"/>
+      <c r="D35" s="111"/>
+      <c r="E35" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="F35" s="69"/>
-      <c r="G35" s="70"/>
+      <c r="F35" s="53"/>
+      <c r="G35" s="54"/>
       <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
-      <c r="B36" s="88"/>
-      <c r="C36" s="89"/>
-      <c r="D36" s="90"/>
-      <c r="E36" s="91" t="s">
+      <c r="B36" s="109"/>
+      <c r="C36" s="110"/>
+      <c r="D36" s="111"/>
+      <c r="E36" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="F36" s="69"/>
-      <c r="G36" s="70"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="54"/>
       <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
-      <c r="B37" s="95" t="s">
+      <c r="B37" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="96"/>
-      <c r="D37" s="97"/>
-      <c r="E37" s="98" t="s">
+      <c r="C37" s="89"/>
+      <c r="D37" s="90"/>
+      <c r="E37" s="91" t="s">
         <v>54</v>
       </c>
-      <c r="F37" s="99"/>
-      <c r="G37" s="100"/>
+      <c r="F37" s="92"/>
+      <c r="G37" s="93"/>
       <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
-      <c r="B38" s="65" t="s">
+      <c r="B38" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="C38" s="66"/>
-      <c r="D38" s="67"/>
-      <c r="E38" s="98"/>
-      <c r="F38" s="99"/>
-      <c r="G38" s="100"/>
+      <c r="C38" s="95"/>
+      <c r="D38" s="96"/>
+      <c r="E38" s="91"/>
+      <c r="F38" s="92"/>
+      <c r="G38" s="93"/>
       <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
-      <c r="B39" s="101" t="s">
+      <c r="B39" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="102"/>
-      <c r="D39" s="103"/>
-      <c r="E39" s="104" t="s">
+      <c r="C39" s="66"/>
+      <c r="D39" s="67"/>
+      <c r="E39" s="97" t="s">
         <v>57</v>
       </c>
-      <c r="F39" s="105"/>
-      <c r="G39" s="106"/>
+      <c r="F39" s="98"/>
+      <c r="G39" s="99"/>
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
-      <c r="B40" s="101"/>
-      <c r="C40" s="102"/>
-      <c r="D40" s="103"/>
-      <c r="E40" s="107" t="s">
+      <c r="B40" s="65"/>
+      <c r="C40" s="66"/>
+      <c r="D40" s="67"/>
+      <c r="E40" s="100" t="s">
         <v>58</v>
       </c>
-      <c r="F40" s="108"/>
-      <c r="G40" s="109"/>
+      <c r="F40" s="101"/>
+      <c r="G40" s="102"/>
       <c r="H40" s="10"/>
     </row>
     <row r="41" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
-      <c r="B41" s="68" t="s">
+      <c r="B41" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="C41" s="69"/>
-      <c r="D41" s="70"/>
-      <c r="E41" s="98" t="s">
+      <c r="C41" s="53"/>
+      <c r="D41" s="54"/>
+      <c r="E41" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="F41" s="99"/>
-      <c r="G41" s="100"/>
+      <c r="F41" s="92"/>
+      <c r="G41" s="93"/>
       <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
-      <c r="B42" s="68" t="s">
+      <c r="B42" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="C42" s="69"/>
-      <c r="D42" s="70"/>
-      <c r="E42" s="98"/>
-      <c r="F42" s="99"/>
-      <c r="G42" s="100"/>
+      <c r="C42" s="53"/>
+      <c r="D42" s="54"/>
+      <c r="E42" s="91"/>
+      <c r="F42" s="92"/>
+      <c r="G42" s="93"/>
       <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
-      <c r="B43" s="68" t="s">
+      <c r="B43" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="C43" s="69"/>
-      <c r="D43" s="70"/>
-      <c r="E43" s="110" t="s">
+      <c r="C43" s="53"/>
+      <c r="D43" s="54"/>
+      <c r="E43" s="103" t="s">
         <v>63</v>
       </c>
-      <c r="F43" s="111"/>
-      <c r="G43" s="112"/>
+      <c r="F43" s="104"/>
+      <c r="G43" s="105"/>
       <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
-      <c r="B44" s="68" t="s">
+      <c r="B44" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="C44" s="69"/>
-      <c r="D44" s="70"/>
-      <c r="E44" s="92"/>
-      <c r="F44" s="93"/>
-      <c r="G44" s="94"/>
+      <c r="C44" s="53"/>
+      <c r="D44" s="54"/>
+      <c r="E44" s="85"/>
+      <c r="F44" s="86"/>
+      <c r="G44" s="87"/>
       <c r="H44" s="10"/>
     </row>
     <row r="45" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
-      <c r="B45" s="68" t="s">
+      <c r="B45" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="C45" s="69"/>
-      <c r="D45" s="70"/>
-      <c r="E45" s="114"/>
-      <c r="F45" s="115"/>
-      <c r="G45" s="116"/>
+      <c r="C45" s="53"/>
+      <c r="D45" s="54"/>
+      <c r="E45" s="55"/>
+      <c r="F45" s="56"/>
+      <c r="G45" s="57"/>
       <c r="H45" s="10"/>
     </row>
     <row r="46" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="61" t="s">
+      <c r="B46" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="C46" s="62"/>
-      <c r="D46" s="62"/>
-      <c r="E46" s="117"/>
-      <c r="F46" s="117"/>
-      <c r="G46" s="118"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="59"/>
+      <c r="E46" s="60"/>
+      <c r="F46" s="60"/>
+      <c r="G46" s="61"/>
       <c r="H46" s="10"/>
     </row>
     <row r="47" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
-      <c r="B47" s="119" t="s">
+      <c r="B47" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="C47" s="120"/>
-      <c r="D47" s="121"/>
-      <c r="E47" s="46" t="s">
+      <c r="C47" s="63"/>
+      <c r="D47" s="64"/>
+      <c r="E47" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="F47" s="47"/>
-      <c r="G47" s="48"/>
+      <c r="F47" s="69"/>
+      <c r="G47" s="70"/>
       <c r="H47" s="10"/>
     </row>
     <row r="48" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
-      <c r="B48" s="101"/>
-      <c r="C48" s="102"/>
-      <c r="D48" s="103"/>
-      <c r="E48" s="122" t="s">
+      <c r="B48" s="65"/>
+      <c r="C48" s="66"/>
+      <c r="D48" s="67"/>
+      <c r="E48" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="F48" s="123"/>
-      <c r="G48" s="124"/>
+      <c r="F48" s="72"/>
+      <c r="G48" s="73"/>
       <c r="H48" s="10"/>
     </row>
     <row r="49" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
-      <c r="B49" s="101"/>
-      <c r="C49" s="102"/>
-      <c r="D49" s="103"/>
-      <c r="E49" s="91" t="s">
+      <c r="B49" s="65"/>
+      <c r="C49" s="66"/>
+      <c r="D49" s="67"/>
+      <c r="E49" s="74" t="s">
         <v>70</v>
       </c>
-      <c r="F49" s="125"/>
-      <c r="G49" s="126"/>
+      <c r="F49" s="75"/>
+      <c r="G49" s="76"/>
       <c r="H49" s="10"/>
     </row>
     <row r="50" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>
-      <c r="B50" s="127" t="s">
+      <c r="B50" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="C50" s="128"/>
-      <c r="D50" s="129"/>
-      <c r="E50" s="130"/>
-      <c r="F50" s="131"/>
-      <c r="G50" s="132"/>
+      <c r="C50" s="78"/>
+      <c r="D50" s="79"/>
+      <c r="E50" s="80"/>
+      <c r="F50" s="81"/>
+      <c r="G50" s="82"/>
       <c r="H50" s="10"/>
     </row>
     <row r="51" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
-      <c r="B51" s="133"/>
-      <c r="C51" s="133"/>
-      <c r="D51" s="133"/>
-      <c r="E51" s="133"/>
-      <c r="F51" s="133"/>
-      <c r="G51" s="133"/>
+      <c r="B51" s="83"/>
+      <c r="C51" s="83"/>
+      <c r="D51" s="83"/>
+      <c r="E51" s="83"/>
+      <c r="F51" s="83"/>
+      <c r="G51" s="83"/>
       <c r="H51" s="10"/>
     </row>
     <row r="52" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -2780,61 +2780,61 @@
       <c r="B52" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C52" s="134"/>
-      <c r="D52" s="134"/>
-      <c r="E52" s="134"/>
-      <c r="F52" s="134"/>
-      <c r="G52" s="134"/>
+      <c r="C52" s="84"/>
+      <c r="D52" s="84"/>
+      <c r="E52" s="84"/>
+      <c r="F52" s="84"/>
+      <c r="G52" s="84"/>
       <c r="H52" s="10"/>
     </row>
     <row r="53" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
-      <c r="B53" s="113"/>
-      <c r="C53" s="113"/>
-      <c r="D53" s="113"/>
-      <c r="E53" s="113"/>
-      <c r="F53" s="113"/>
-      <c r="G53" s="113"/>
+      <c r="B53" s="51"/>
+      <c r="C53" s="51"/>
+      <c r="D53" s="51"/>
+      <c r="E53" s="51"/>
+      <c r="F53" s="51"/>
+      <c r="G53" s="51"/>
       <c r="H53" s="10"/>
     </row>
     <row r="54" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
-      <c r="B54" s="113"/>
-      <c r="C54" s="113"/>
-      <c r="D54" s="113"/>
-      <c r="E54" s="113"/>
-      <c r="F54" s="113"/>
-      <c r="G54" s="113"/>
+      <c r="B54" s="51"/>
+      <c r="C54" s="51"/>
+      <c r="D54" s="51"/>
+      <c r="E54" s="51"/>
+      <c r="F54" s="51"/>
+      <c r="G54" s="51"/>
       <c r="H54" s="10"/>
     </row>
     <row r="55" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
-      <c r="B55" s="135"/>
-      <c r="C55" s="135"/>
-      <c r="D55" s="135"/>
-      <c r="E55" s="135"/>
-      <c r="F55" s="135"/>
-      <c r="G55" s="135"/>
+      <c r="B55" s="47"/>
+      <c r="C55" s="47"/>
+      <c r="D55" s="47"/>
+      <c r="E55" s="47"/>
+      <c r="F55" s="47"/>
+      <c r="G55" s="47"/>
       <c r="H55" s="10"/>
     </row>
     <row r="56" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="21"/>
-      <c r="B56" s="136" t="s">
+      <c r="B56" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="C56" s="136"/>
-      <c r="D56" s="136"/>
-      <c r="E56" s="136"/>
-      <c r="F56" s="136"/>
-      <c r="G56" s="136"/>
+      <c r="C56" s="43"/>
+      <c r="D56" s="43"/>
+      <c r="E56" s="43"/>
+      <c r="F56" s="43"/>
+      <c r="G56" s="43"/>
       <c r="H56" s="22"/>
     </row>
     <row r="57" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="22"/>
-      <c r="B57" s="137" t="s">
+      <c r="B57" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="C57" s="137"/>
+      <c r="C57" s="48"/>
       <c r="D57" s="32">
         <v>7</v>
       </c>
@@ -2847,135 +2847,135 @@
     </row>
     <row r="58" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="21"/>
-      <c r="B58" s="136" t="s">
+      <c r="B58" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="C58" s="136"/>
-      <c r="D58" s="136"/>
-      <c r="E58" s="136"/>
-      <c r="F58" s="136"/>
-      <c r="G58" s="136"/>
+      <c r="C58" s="43"/>
+      <c r="D58" s="43"/>
+      <c r="E58" s="43"/>
+      <c r="F58" s="43"/>
+      <c r="G58" s="43"/>
       <c r="H58" s="22"/>
     </row>
     <row r="59" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="22"/>
-      <c r="B59" s="138" t="s">
+      <c r="B59" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="C59" s="138"/>
+      <c r="C59" s="49"/>
       <c r="D59" s="33">
         <f>SUM(C61:C61)</f>
         <v>0</v>
       </c>
-      <c r="E59" s="139" t="s">
+      <c r="E59" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="F59" s="139"/>
+      <c r="F59" s="50"/>
       <c r="G59" s="20"/>
       <c r="H59" s="22"/>
     </row>
     <row r="60" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="21"/>
-      <c r="B60" s="136" t="s">
+      <c r="B60" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="C60" s="136"/>
-      <c r="D60" s="136"/>
-      <c r="E60" s="136"/>
-      <c r="F60" s="136"/>
-      <c r="G60" s="136"/>
+      <c r="C60" s="43"/>
+      <c r="D60" s="43"/>
+      <c r="E60" s="43"/>
+      <c r="F60" s="43"/>
+      <c r="G60" s="43"/>
       <c r="H60" s="22"/>
     </row>
     <row r="61" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="22"/>
       <c r="B61" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="C61" s="35"/>
+      <c r="D61" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="C61" s="35"/>
-      <c r="D61" s="140" t="s">
-        <v>81</v>
-      </c>
-      <c r="E61" s="140"/>
-      <c r="F61" s="140"/>
+      <c r="E61" s="44"/>
+      <c r="F61" s="44"/>
       <c r="G61" s="36">
         <f ca="1">E17</f>
-        <v>45827</v>
+        <v>45838</v>
       </c>
       <c r="H61" s="22"/>
     </row>
     <row r="62" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
-      <c r="B62" s="141" t="s">
-        <v>82</v>
-      </c>
-      <c r="C62" s="141"/>
-      <c r="D62" s="141"/>
-      <c r="E62" s="141"/>
-      <c r="F62" s="141"/>
-      <c r="G62" s="141"/>
+      <c r="B62" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="C62" s="45"/>
+      <c r="D62" s="45"/>
+      <c r="E62" s="45"/>
+      <c r="F62" s="45"/>
+      <c r="G62" s="45"/>
       <c r="H62" s="37"/>
     </row>
     <row r="63" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="B63" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="B63" s="142" t="s">
+      <c r="C63" s="46"/>
+      <c r="D63" s="46"/>
+      <c r="E63" s="46"/>
+      <c r="F63" s="46"/>
+      <c r="G63" s="46"/>
+    </row>
+    <row r="64" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="C63" s="142"/>
-      <c r="D63" s="142"/>
-      <c r="E63" s="142"/>
-      <c r="F63" s="142"/>
-      <c r="G63" s="142"/>
-    </row>
-    <row r="64" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="143" t="s">
+      <c r="C64" s="42"/>
+      <c r="D64" s="42"/>
+      <c r="E64" s="42"/>
+      <c r="F64" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="C64" s="143"/>
-      <c r="D64" s="143"/>
-      <c r="E64" s="143"/>
-      <c r="F64" s="143" t="s">
+      <c r="G64" s="42"/>
+      <c r="H64" s="42"/>
+    </row>
+    <row r="65" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="G64" s="143"/>
-      <c r="H64" s="143"/>
-    </row>
-    <row r="65" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="144" t="s">
+      <c r="C65" s="41"/>
+      <c r="D65" s="41"/>
+      <c r="E65" s="41"/>
+      <c r="F65" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="C65" s="144"/>
-      <c r="D65" s="144"/>
-      <c r="E65" s="144"/>
-      <c r="F65" s="143" t="s">
+      <c r="G65" s="42"/>
+      <c r="H65" s="42"/>
+    </row>
+    <row r="66" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="G65" s="143"/>
-      <c r="H65" s="143"/>
-    </row>
-    <row r="66" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="144" t="s">
+      <c r="C66" s="41"/>
+      <c r="D66" s="41"/>
+      <c r="E66" s="41"/>
+      <c r="F66" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="C66" s="144"/>
-      <c r="D66" s="144"/>
-      <c r="E66" s="144"/>
-      <c r="F66" s="143" t="s">
+      <c r="G66" s="42"/>
+      <c r="H66" s="42"/>
+    </row>
+    <row r="67" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="G66" s="143"/>
-      <c r="H66" s="143"/>
-    </row>
-    <row r="67" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="143" t="s">
-        <v>91</v>
-      </c>
-      <c r="C67" s="143"/>
-      <c r="D67" s="143"/>
-      <c r="E67" s="143"/>
-      <c r="F67" s="143"/>
-      <c r="G67" s="143"/>
+      <c r="C67" s="42"/>
+      <c r="D67" s="42"/>
+      <c r="E67" s="42"/>
+      <c r="F67" s="42"/>
+      <c r="G67" s="42"/>
     </row>
     <row r="68" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="39"/>
@@ -3005,24 +3005,63 @@
     <protectedRange algorithmName="SHA-512" hashValue="1IwEtpPovyRjspz9ti3J5udl070IPZ9gDlGmM3ZH/lFyQlLVVL2qbaMds7kHvZZkPq7VvowLV2MqpNnf8owpjQ==" saltValue="SwYyjj//I75seGLqQP0hyQ==" spinCount="100000" sqref="E37:G38 E39" name="Rango2_2"/>
   </protectedRanges>
   <mergeCells count="88">
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="B66:E66"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="B62:G62"/>
-    <mergeCell ref="B63:G63"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="B55:G55"/>
-    <mergeCell ref="B56:G56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:G58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="B9:G10"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="B32:D33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="B35:D36"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:G38"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B39:D40"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="E41:G42"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="E43:G43"/>
     <mergeCell ref="B54:G54"/>
     <mergeCell ref="B45:D45"/>
     <mergeCell ref="E45:G45"/>
@@ -3036,63 +3075,24 @@
     <mergeCell ref="B51:G51"/>
     <mergeCell ref="C52:G52"/>
     <mergeCell ref="B53:G53"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E37:G38"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B39:D40"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="E41:G42"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="B32:D33"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="B35:D36"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="B9:G10"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="B56:G56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="B62:G62"/>
+    <mergeCell ref="B63:G63"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="B66:E66"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="F67:G67"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D7" r:id="rId1" xr:uid="{06F8AEE0-B467-46CC-BA80-3945E484B37D}"/>

</xml_diff>

<commit_message>
feat: se cambio nombre de ing verificador
</commit_message>
<xml_diff>
--- a/backend/docs/ACT-AUT.xlsx
+++ b/backend/docs/ACT-AUT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\planosperu-app\backend\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FF0D8D-8479-4346-AB6D-48E419609CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85DA608-524C-45C5-A3D8-613454931241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{96D1BB80-F449-4442-8AAB-F71CF7F38B12}"/>
   </bookViews>
@@ -293,9 +293,6 @@
     <t>STAFF DE PROFESIONALES:</t>
   </si>
   <si>
-    <t>Ing. Santillan Quiroz Julio  Nº CIP:56827  CIV: 022023VCZRIX</t>
-  </si>
-  <si>
     <t>Abog.Ljubica Nada Sékula Delgado CAD 18346</t>
   </si>
   <si>
@@ -315,6 +312,9 @@
   </si>
   <si>
     <t xml:space="preserve">Cuota 1 S/  </t>
+  </si>
+  <si>
+    <t>Ing. Aguirre Alanya Luis Antonio CIP: 323997 CIV: 022178VCZRIX</t>
   </si>
 </sst>
 </file>
@@ -804,42 +804,104 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -853,114 +915,87 @@
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -991,16 +1026,16 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1030,153 +1065,118 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2146,8 +2146,8 @@
   </sheetPr>
   <dimension ref="A3:H78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A46" zoomScale="130" zoomScaleNormal="50" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64:E64"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A60" zoomScale="130" zoomScaleNormal="50" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66:E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2169,86 +2169,86 @@
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="141" t="s">
+      <c r="D4" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="141"/>
-      <c r="F4" s="141"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="142" t="s">
+      <c r="D5" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="142"/>
-      <c r="F5" s="142"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="143" t="s">
+      <c r="D6" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="143"/>
-      <c r="F6" s="143"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="144" t="s">
+      <c r="D7" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="144"/>
-      <c r="F7" s="144"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="145"/>
-      <c r="B8" s="145"/>
-      <c r="C8" s="145"/>
-      <c r="D8" s="145"/>
-      <c r="E8" s="145"/>
-      <c r="F8" s="145"/>
-      <c r="G8" s="145"/>
-      <c r="H8" s="145"/>
+      <c r="A8" s="46"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
     </row>
     <row r="9" spans="1:8" s="5" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="140" t="s">
+      <c r="B9" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="140"/>
-      <c r="D9" s="140"/>
-      <c r="E9" s="140"/>
-      <c r="F9" s="140"/>
-      <c r="G9" s="140"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:8" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="140"/>
-      <c r="C10" s="140"/>
-      <c r="D10" s="140"/>
-      <c r="E10" s="140"/>
-      <c r="F10" s="140"/>
-      <c r="G10" s="140"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="128" t="s">
+      <c r="B11" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="128"/>
-      <c r="D11" s="128"/>
-      <c r="E11" s="128"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
       <c r="F11" s="8" t="s">
         <v>12</v>
       </c>
@@ -2257,22 +2257,22 @@
     </row>
     <row r="12" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="128"/>
-      <c r="C12" s="128"/>
-      <c r="D12" s="128"/>
-      <c r="E12" s="128"/>
-      <c r="F12" s="128"/>
-      <c r="G12" s="128"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
-      <c r="B13" s="128"/>
-      <c r="C13" s="128"/>
-      <c r="D13" s="128"/>
-      <c r="E13" s="128"/>
-      <c r="F13" s="128"/>
-      <c r="G13" s="128"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -2297,10 +2297,10 @@
       <c r="A15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="128"/>
-      <c r="C15" s="128"/>
-      <c r="D15" s="128"/>
-      <c r="E15" s="128"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
       <c r="F15" s="13" t="s">
         <v>18</v>
       </c>
@@ -2309,10 +2309,10 @@
     </row>
     <row r="16" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
-      <c r="B16" s="129"/>
-      <c r="C16" s="129"/>
-      <c r="D16" s="129"/>
-      <c r="E16" s="129"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
       <c r="F16" s="13" t="s">
         <v>19</v>
       </c>
@@ -2323,8 +2323,8 @@
       <c r="A17" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="128"/>
-      <c r="C17" s="128"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
       <c r="D17" s="18" t="s">
         <v>21</v>
       </c>
@@ -2338,183 +2338,183 @@
     </row>
     <row r="18" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
-      <c r="B18" s="130"/>
-      <c r="C18" s="130"/>
-      <c r="D18" s="130"/>
-      <c r="E18" s="130"/>
-      <c r="F18" s="130"/>
-      <c r="G18" s="130"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
       <c r="H18" s="20"/>
     </row>
     <row r="19" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
-      <c r="B19" s="131" t="s">
+      <c r="B19" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="132"/>
-      <c r="D19" s="133"/>
-      <c r="E19" s="134"/>
-      <c r="F19" s="134"/>
-      <c r="G19" s="134"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="56"/>
       <c r="H19" s="22"/>
     </row>
     <row r="20" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
-      <c r="B20" s="135" t="s">
+      <c r="B20" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="136"/>
-      <c r="D20" s="137"/>
-      <c r="E20" s="138" t="s">
+      <c r="C20" s="58"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="138"/>
-      <c r="G20" s="139"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="61"/>
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
-      <c r="B21" s="68" t="s">
+      <c r="B21" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="69"/>
-      <c r="D21" s="70"/>
-      <c r="E21" s="69" t="s">
+      <c r="C21" s="48"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="F21" s="69"/>
-      <c r="G21" s="70"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="49"/>
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
-      <c r="B22" s="58" t="s">
+      <c r="B22" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="59"/>
-      <c r="D22" s="59"/>
-      <c r="E22" s="126"/>
-      <c r="F22" s="126"/>
-      <c r="G22" s="127"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="65"/>
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
-      <c r="B23" s="68" t="s">
+      <c r="B23" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="69"/>
-      <c r="D23" s="70"/>
-      <c r="E23" s="68" t="s">
+      <c r="C23" s="48"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="69"/>
-      <c r="G23" s="70"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="49"/>
       <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
-      <c r="B24" s="68" t="s">
+      <c r="B24" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="69"/>
-      <c r="D24" s="70"/>
-      <c r="E24" s="68" t="s">
+      <c r="C24" s="48"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="F24" s="69"/>
-      <c r="G24" s="70"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="49"/>
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="24"/>
-      <c r="B25" s="68" t="s">
+      <c r="B25" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="69"/>
-      <c r="D25" s="70"/>
-      <c r="E25" s="68" t="s">
+      <c r="C25" s="48"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="69"/>
-      <c r="G25" s="70"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="49"/>
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="25"/>
-      <c r="B26" s="68" t="s">
+      <c r="B26" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="69"/>
-      <c r="D26" s="70"/>
-      <c r="E26" s="68" t="s">
+      <c r="C26" s="48"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="F26" s="69"/>
-      <c r="G26" s="70"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="49"/>
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="25"/>
-      <c r="B27" s="52" t="s">
+      <c r="B27" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="53"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="68" t="s">
+      <c r="C27" s="70"/>
+      <c r="D27" s="71"/>
+      <c r="E27" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="69"/>
-      <c r="G27" s="70"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="49"/>
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="25"/>
-      <c r="B28" s="112" t="s">
+      <c r="B28" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="113"/>
-      <c r="D28" s="114"/>
-      <c r="E28" s="115" t="s">
+      <c r="C28" s="73"/>
+      <c r="D28" s="74"/>
+      <c r="E28" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="F28" s="116"/>
-      <c r="G28" s="117"/>
+      <c r="F28" s="76"/>
+      <c r="G28" s="77"/>
       <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="25"/>
-      <c r="B29" s="58" t="s">
+      <c r="B29" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="59"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="118"/>
-      <c r="F29" s="118"/>
-      <c r="G29" s="119"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="78"/>
+      <c r="F29" s="78"/>
+      <c r="G29" s="79"/>
       <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="26"/>
-      <c r="B30" s="120" t="s">
+      <c r="B30" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="121"/>
-      <c r="D30" s="122"/>
-      <c r="E30" s="123" t="s">
+      <c r="C30" s="81"/>
+      <c r="D30" s="82"/>
+      <c r="E30" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="F30" s="124"/>
-      <c r="G30" s="125"/>
+      <c r="F30" s="84"/>
+      <c r="G30" s="85"/>
       <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="26"/>
-      <c r="B31" s="94" t="s">
+      <c r="B31" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="95"/>
-      <c r="D31" s="96"/>
+      <c r="C31" s="67"/>
+      <c r="D31" s="68"/>
       <c r="E31" s="27" t="s">
         <v>44</v>
       </c>
@@ -2524,11 +2524,11 @@
     </row>
     <row r="32" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="30"/>
-      <c r="B32" s="106" t="s">
+      <c r="B32" s="86" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="107"/>
-      <c r="D32" s="108"/>
+      <c r="C32" s="87"/>
+      <c r="D32" s="88"/>
       <c r="E32" s="27" t="s">
         <v>46</v>
       </c>
@@ -2538,241 +2538,241 @@
     </row>
     <row r="33" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
-      <c r="B33" s="106"/>
-      <c r="C33" s="107"/>
-      <c r="D33" s="108"/>
-      <c r="E33" s="52" t="s">
+      <c r="B33" s="86"/>
+      <c r="C33" s="87"/>
+      <c r="D33" s="88"/>
+      <c r="E33" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="F33" s="53"/>
-      <c r="G33" s="54"/>
+      <c r="F33" s="70"/>
+      <c r="G33" s="71"/>
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
-      <c r="B34" s="52" t="s">
+      <c r="B34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="53"/>
-      <c r="D34" s="54"/>
-      <c r="E34" s="52" t="s">
+      <c r="C34" s="70"/>
+      <c r="D34" s="71"/>
+      <c r="E34" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="F34" s="53"/>
-      <c r="G34" s="54"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="71"/>
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
-      <c r="B35" s="109" t="s">
+      <c r="B35" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="110"/>
-      <c r="D35" s="111"/>
-      <c r="E35" s="52" t="s">
+      <c r="C35" s="90"/>
+      <c r="D35" s="91"/>
+      <c r="E35" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="F35" s="53"/>
-      <c r="G35" s="54"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="71"/>
       <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
-      <c r="B36" s="109"/>
-      <c r="C36" s="110"/>
-      <c r="D36" s="111"/>
-      <c r="E36" s="74" t="s">
+      <c r="B36" s="89"/>
+      <c r="C36" s="90"/>
+      <c r="D36" s="91"/>
+      <c r="E36" s="92" t="s">
         <v>52</v>
       </c>
-      <c r="F36" s="53"/>
-      <c r="G36" s="54"/>
+      <c r="F36" s="70"/>
+      <c r="G36" s="71"/>
       <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
-      <c r="B37" s="88" t="s">
+      <c r="B37" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="89"/>
-      <c r="D37" s="90"/>
-      <c r="E37" s="91" t="s">
+      <c r="C37" s="97"/>
+      <c r="D37" s="98"/>
+      <c r="E37" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="F37" s="92"/>
-      <c r="G37" s="93"/>
+      <c r="F37" s="100"/>
+      <c r="G37" s="101"/>
       <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
-      <c r="B38" s="94" t="s">
+      <c r="B38" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="C38" s="95"/>
-      <c r="D38" s="96"/>
-      <c r="E38" s="91"/>
-      <c r="F38" s="92"/>
-      <c r="G38" s="93"/>
+      <c r="C38" s="67"/>
+      <c r="D38" s="68"/>
+      <c r="E38" s="99"/>
+      <c r="F38" s="100"/>
+      <c r="G38" s="101"/>
       <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
-      <c r="B39" s="65" t="s">
+      <c r="B39" s="102" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="66"/>
-      <c r="D39" s="67"/>
-      <c r="E39" s="97" t="s">
+      <c r="C39" s="103"/>
+      <c r="D39" s="104"/>
+      <c r="E39" s="105" t="s">
         <v>57</v>
       </c>
-      <c r="F39" s="98"/>
-      <c r="G39" s="99"/>
+      <c r="F39" s="106"/>
+      <c r="G39" s="107"/>
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
-      <c r="B40" s="65"/>
-      <c r="C40" s="66"/>
-      <c r="D40" s="67"/>
-      <c r="E40" s="100" t="s">
+      <c r="B40" s="102"/>
+      <c r="C40" s="103"/>
+      <c r="D40" s="104"/>
+      <c r="E40" s="108" t="s">
         <v>58</v>
       </c>
-      <c r="F40" s="101"/>
-      <c r="G40" s="102"/>
+      <c r="F40" s="109"/>
+      <c r="G40" s="110"/>
       <c r="H40" s="10"/>
     </row>
     <row r="41" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
-      <c r="B41" s="52" t="s">
+      <c r="B41" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="C41" s="53"/>
-      <c r="D41" s="54"/>
-      <c r="E41" s="91" t="s">
+      <c r="C41" s="70"/>
+      <c r="D41" s="71"/>
+      <c r="E41" s="99" t="s">
         <v>60</v>
       </c>
-      <c r="F41" s="92"/>
-      <c r="G41" s="93"/>
+      <c r="F41" s="100"/>
+      <c r="G41" s="101"/>
       <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
-      <c r="B42" s="52" t="s">
+      <c r="B42" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="C42" s="53"/>
-      <c r="D42" s="54"/>
-      <c r="E42" s="91"/>
-      <c r="F42" s="92"/>
-      <c r="G42" s="93"/>
+      <c r="C42" s="70"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="99"/>
+      <c r="F42" s="100"/>
+      <c r="G42" s="101"/>
       <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
-      <c r="B43" s="52" t="s">
+      <c r="B43" s="69" t="s">
         <v>62</v>
       </c>
-      <c r="C43" s="53"/>
-      <c r="D43" s="54"/>
-      <c r="E43" s="103" t="s">
+      <c r="C43" s="70"/>
+      <c r="D43" s="71"/>
+      <c r="E43" s="111" t="s">
         <v>63</v>
       </c>
-      <c r="F43" s="104"/>
-      <c r="G43" s="105"/>
+      <c r="F43" s="112"/>
+      <c r="G43" s="113"/>
       <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
-      <c r="B44" s="52" t="s">
+      <c r="B44" s="69" t="s">
         <v>64</v>
       </c>
-      <c r="C44" s="53"/>
-      <c r="D44" s="54"/>
-      <c r="E44" s="85"/>
-      <c r="F44" s="86"/>
-      <c r="G44" s="87"/>
+      <c r="C44" s="70"/>
+      <c r="D44" s="71"/>
+      <c r="E44" s="93"/>
+      <c r="F44" s="94"/>
+      <c r="G44" s="95"/>
       <c r="H44" s="10"/>
     </row>
     <row r="45" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
-      <c r="B45" s="52" t="s">
+      <c r="B45" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="C45" s="53"/>
-      <c r="D45" s="54"/>
-      <c r="E45" s="55"/>
-      <c r="F45" s="56"/>
-      <c r="G45" s="57"/>
+      <c r="C45" s="70"/>
+      <c r="D45" s="71"/>
+      <c r="E45" s="115"/>
+      <c r="F45" s="116"/>
+      <c r="G45" s="117"/>
       <c r="H45" s="10"/>
     </row>
     <row r="46" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="58" t="s">
+      <c r="B46" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="C46" s="59"/>
-      <c r="D46" s="59"/>
-      <c r="E46" s="60"/>
-      <c r="F46" s="60"/>
-      <c r="G46" s="61"/>
+      <c r="C46" s="63"/>
+      <c r="D46" s="63"/>
+      <c r="E46" s="118"/>
+      <c r="F46" s="118"/>
+      <c r="G46" s="119"/>
       <c r="H46" s="10"/>
     </row>
     <row r="47" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
-      <c r="B47" s="62" t="s">
+      <c r="B47" s="120" t="s">
         <v>67</v>
       </c>
-      <c r="C47" s="63"/>
-      <c r="D47" s="64"/>
-      <c r="E47" s="68" t="s">
+      <c r="C47" s="121"/>
+      <c r="D47" s="122"/>
+      <c r="E47" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="F47" s="69"/>
-      <c r="G47" s="70"/>
+      <c r="F47" s="48"/>
+      <c r="G47" s="49"/>
       <c r="H47" s="10"/>
     </row>
     <row r="48" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
-      <c r="B48" s="65"/>
-      <c r="C48" s="66"/>
-      <c r="D48" s="67"/>
-      <c r="E48" s="71" t="s">
+      <c r="B48" s="102"/>
+      <c r="C48" s="103"/>
+      <c r="D48" s="104"/>
+      <c r="E48" s="123" t="s">
         <v>69</v>
       </c>
-      <c r="F48" s="72"/>
-      <c r="G48" s="73"/>
+      <c r="F48" s="124"/>
+      <c r="G48" s="125"/>
       <c r="H48" s="10"/>
     </row>
     <row r="49" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
-      <c r="B49" s="65"/>
-      <c r="C49" s="66"/>
-      <c r="D49" s="67"/>
-      <c r="E49" s="74" t="s">
+      <c r="B49" s="102"/>
+      <c r="C49" s="103"/>
+      <c r="D49" s="104"/>
+      <c r="E49" s="92" t="s">
         <v>70</v>
       </c>
-      <c r="F49" s="75"/>
-      <c r="G49" s="76"/>
+      <c r="F49" s="126"/>
+      <c r="G49" s="127"/>
       <c r="H49" s="10"/>
     </row>
     <row r="50" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>
-      <c r="B50" s="77" t="s">
+      <c r="B50" s="128" t="s">
         <v>71</v>
       </c>
-      <c r="C50" s="78"/>
-      <c r="D50" s="79"/>
-      <c r="E50" s="80"/>
-      <c r="F50" s="81"/>
-      <c r="G50" s="82"/>
+      <c r="C50" s="129"/>
+      <c r="D50" s="130"/>
+      <c r="E50" s="131"/>
+      <c r="F50" s="132"/>
+      <c r="G50" s="133"/>
       <c r="H50" s="10"/>
     </row>
     <row r="51" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
-      <c r="B51" s="83"/>
-      <c r="C51" s="83"/>
-      <c r="D51" s="83"/>
-      <c r="E51" s="83"/>
-      <c r="F51" s="83"/>
-      <c r="G51" s="83"/>
+      <c r="B51" s="134"/>
+      <c r="C51" s="134"/>
+      <c r="D51" s="134"/>
+      <c r="E51" s="134"/>
+      <c r="F51" s="134"/>
+      <c r="G51" s="134"/>
       <c r="H51" s="10"/>
     </row>
     <row r="52" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -2780,61 +2780,61 @@
       <c r="B52" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C52" s="84"/>
-      <c r="D52" s="84"/>
-      <c r="E52" s="84"/>
-      <c r="F52" s="84"/>
-      <c r="G52" s="84"/>
+      <c r="C52" s="135"/>
+      <c r="D52" s="135"/>
+      <c r="E52" s="135"/>
+      <c r="F52" s="135"/>
+      <c r="G52" s="135"/>
       <c r="H52" s="10"/>
     </row>
     <row r="53" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
-      <c r="B53" s="51"/>
-      <c r="C53" s="51"/>
-      <c r="D53" s="51"/>
-      <c r="E53" s="51"/>
-      <c r="F53" s="51"/>
-      <c r="G53" s="51"/>
+      <c r="B53" s="114"/>
+      <c r="C53" s="114"/>
+      <c r="D53" s="114"/>
+      <c r="E53" s="114"/>
+      <c r="F53" s="114"/>
+      <c r="G53" s="114"/>
       <c r="H53" s="10"/>
     </row>
     <row r="54" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
-      <c r="B54" s="51"/>
-      <c r="C54" s="51"/>
-      <c r="D54" s="51"/>
-      <c r="E54" s="51"/>
-      <c r="F54" s="51"/>
-      <c r="G54" s="51"/>
+      <c r="B54" s="114"/>
+      <c r="C54" s="114"/>
+      <c r="D54" s="114"/>
+      <c r="E54" s="114"/>
+      <c r="F54" s="114"/>
+      <c r="G54" s="114"/>
       <c r="H54" s="10"/>
     </row>
     <row r="55" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
-      <c r="B55" s="47"/>
-      <c r="C55" s="47"/>
-      <c r="D55" s="47"/>
-      <c r="E55" s="47"/>
-      <c r="F55" s="47"/>
-      <c r="G55" s="47"/>
+      <c r="B55" s="136"/>
+      <c r="C55" s="136"/>
+      <c r="D55" s="136"/>
+      <c r="E55" s="136"/>
+      <c r="F55" s="136"/>
+      <c r="G55" s="136"/>
       <c r="H55" s="10"/>
     </row>
     <row r="56" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="21"/>
-      <c r="B56" s="43" t="s">
+      <c r="B56" s="137" t="s">
         <v>73</v>
       </c>
-      <c r="C56" s="43"/>
-      <c r="D56" s="43"/>
-      <c r="E56" s="43"/>
-      <c r="F56" s="43"/>
-      <c r="G56" s="43"/>
+      <c r="C56" s="137"/>
+      <c r="D56" s="137"/>
+      <c r="E56" s="137"/>
+      <c r="F56" s="137"/>
+      <c r="G56" s="137"/>
       <c r="H56" s="22"/>
     </row>
     <row r="57" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="22"/>
-      <c r="B57" s="48" t="s">
+      <c r="B57" s="138" t="s">
         <v>74</v>
       </c>
-      <c r="C57" s="48"/>
+      <c r="C57" s="138"/>
       <c r="D57" s="32">
         <v>7</v>
       </c>
@@ -2847,56 +2847,56 @@
     </row>
     <row r="58" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="21"/>
-      <c r="B58" s="43" t="s">
+      <c r="B58" s="137" t="s">
         <v>76</v>
       </c>
-      <c r="C58" s="43"/>
-      <c r="D58" s="43"/>
-      <c r="E58" s="43"/>
-      <c r="F58" s="43"/>
-      <c r="G58" s="43"/>
+      <c r="C58" s="137"/>
+      <c r="D58" s="137"/>
+      <c r="E58" s="137"/>
+      <c r="F58" s="137"/>
+      <c r="G58" s="137"/>
       <c r="H58" s="22"/>
     </row>
     <row r="59" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="22"/>
-      <c r="B59" s="49" t="s">
+      <c r="B59" s="139" t="s">
         <v>77</v>
       </c>
-      <c r="C59" s="49"/>
+      <c r="C59" s="139"/>
       <c r="D59" s="33">
         <f>SUM(C61:C61)</f>
         <v>0</v>
       </c>
-      <c r="E59" s="50" t="s">
+      <c r="E59" s="140" t="s">
         <v>78</v>
       </c>
-      <c r="F59" s="50"/>
+      <c r="F59" s="140"/>
       <c r="G59" s="20"/>
       <c r="H59" s="22"/>
     </row>
     <row r="60" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="21"/>
-      <c r="B60" s="43" t="s">
+      <c r="B60" s="137" t="s">
         <v>79</v>
       </c>
-      <c r="C60" s="43"/>
-      <c r="D60" s="43"/>
-      <c r="E60" s="43"/>
-      <c r="F60" s="43"/>
-      <c r="G60" s="43"/>
+      <c r="C60" s="137"/>
+      <c r="D60" s="137"/>
+      <c r="E60" s="137"/>
+      <c r="F60" s="137"/>
+      <c r="G60" s="137"/>
       <c r="H60" s="22"/>
     </row>
     <row r="61" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="22"/>
       <c r="B61" s="34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C61" s="35"/>
-      <c r="D61" s="44" t="s">
+      <c r="D61" s="141" t="s">
         <v>80</v>
       </c>
-      <c r="E61" s="44"/>
-      <c r="F61" s="44"/>
+      <c r="E61" s="141"/>
+      <c r="F61" s="141"/>
       <c r="G61" s="36">
         <f ca="1">E17</f>
         <v>45838</v>
@@ -2905,77 +2905,77 @@
     </row>
     <row r="62" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
-      <c r="B62" s="45" t="s">
+      <c r="B62" s="142" t="s">
         <v>81</v>
       </c>
-      <c r="C62" s="45"/>
-      <c r="D62" s="45"/>
-      <c r="E62" s="45"/>
-      <c r="F62" s="45"/>
-      <c r="G62" s="45"/>
+      <c r="C62" s="142"/>
+      <c r="D62" s="142"/>
+      <c r="E62" s="142"/>
+      <c r="F62" s="142"/>
+      <c r="G62" s="142"/>
       <c r="H62" s="37"/>
     </row>
     <row r="63" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="B63" s="46" t="s">
+      <c r="B63" s="143" t="s">
         <v>83</v>
       </c>
-      <c r="C63" s="46"/>
-      <c r="D63" s="46"/>
-      <c r="E63" s="46"/>
-      <c r="F63" s="46"/>
-      <c r="G63" s="46"/>
+      <c r="C63" s="143"/>
+      <c r="D63" s="143"/>
+      <c r="E63" s="143"/>
+      <c r="F63" s="143"/>
+      <c r="G63" s="143"/>
     </row>
     <row r="64" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="42" t="s">
+      <c r="B64" s="144" t="s">
+        <v>91</v>
+      </c>
+      <c r="C64" s="144"/>
+      <c r="D64" s="144"/>
+      <c r="E64" s="144"/>
+      <c r="F64" s="144" t="s">
         <v>84</v>
       </c>
-      <c r="C64" s="42"/>
-      <c r="D64" s="42"/>
-      <c r="E64" s="42"/>
-      <c r="F64" s="42" t="s">
+      <c r="G64" s="144"/>
+      <c r="H64" s="144"/>
+    </row>
+    <row r="65" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="145" t="s">
         <v>85</v>
       </c>
-      <c r="G64" s="42"/>
-      <c r="H64" s="42"/>
-    </row>
-    <row r="65" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="41" t="s">
+      <c r="C65" s="145"/>
+      <c r="D65" s="145"/>
+      <c r="E65" s="145"/>
+      <c r="F65" s="144" t="s">
         <v>86</v>
       </c>
-      <c r="C65" s="41"/>
-      <c r="D65" s="41"/>
-      <c r="E65" s="41"/>
-      <c r="F65" s="42" t="s">
+      <c r="G65" s="144"/>
+      <c r="H65" s="144"/>
+    </row>
+    <row r="66" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="145" t="s">
         <v>87</v>
       </c>
-      <c r="G65" s="42"/>
-      <c r="H65" s="42"/>
-    </row>
-    <row r="66" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="41" t="s">
+      <c r="C66" s="145"/>
+      <c r="D66" s="145"/>
+      <c r="E66" s="145"/>
+      <c r="F66" s="144" t="s">
         <v>88</v>
       </c>
-      <c r="C66" s="41"/>
-      <c r="D66" s="41"/>
-      <c r="E66" s="41"/>
-      <c r="F66" s="42" t="s">
+      <c r="G66" s="144"/>
+      <c r="H66" s="144"/>
+    </row>
+    <row r="67" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="144" t="s">
         <v>89</v>
       </c>
-      <c r="G66" s="42"/>
-      <c r="H66" s="42"/>
-    </row>
-    <row r="67" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="42" t="s">
-        <v>90</v>
-      </c>
-      <c r="C67" s="42"/>
-      <c r="D67" s="42"/>
-      <c r="E67" s="42"/>
-      <c r="F67" s="42"/>
-      <c r="G67" s="42"/>
+      <c r="C67" s="144"/>
+      <c r="D67" s="144"/>
+      <c r="E67" s="144"/>
+      <c r="F67" s="144"/>
+      <c r="G67" s="144"/>
     </row>
     <row r="68" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="39"/>
@@ -3005,12 +3005,75 @@
     <protectedRange algorithmName="SHA-512" hashValue="1IwEtpPovyRjspz9ti3J5udl070IPZ9gDlGmM3ZH/lFyQlLVVL2qbaMds7kHvZZkPq7VvowLV2MqpNnf8owpjQ==" saltValue="SwYyjj//I75seGLqQP0hyQ==" spinCount="100000" sqref="E37:G38 E39" name="Rango2_2"/>
   </protectedRanges>
   <mergeCells count="88">
-    <mergeCell ref="B9:G10"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="B66:E66"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="B62:G62"/>
+    <mergeCell ref="B63:G63"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="B56:G56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="B47:D49"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="C52:G52"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:G38"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B39:D40"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="E41:G42"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="B32:D33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="B35:D36"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:G24"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="E21:G21"/>
     <mergeCell ref="B11:E11"/>
@@ -3024,75 +3087,12 @@
     <mergeCell ref="E19:G19"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="E20:G20"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="B32:D33"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="B35:D36"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E37:G38"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B39:D40"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="E41:G42"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="B54:G54"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="B46:G46"/>
-    <mergeCell ref="B47:D49"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="C52:G52"/>
-    <mergeCell ref="B53:G53"/>
-    <mergeCell ref="B55:G55"/>
-    <mergeCell ref="B56:G56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:G58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="B62:G62"/>
-    <mergeCell ref="B63:G63"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="B66:E66"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="B9:G10"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="A8:H8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D7" r:id="rId1" xr:uid="{06F8AEE0-B467-46CC-BA80-3945E484B37D}"/>

</xml_diff>

<commit_message>
feat: la reconcha de su madre me olvide el Pisos
</commit_message>
<xml_diff>
--- a/backend/docs/ACT-AUT.xlsx
+++ b/backend/docs/ACT-AUT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\planosperu-app\backend\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85DA608-524C-45C5-A3D8-613454931241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D2E014-5600-470F-B7E6-EC1170E9FF1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{96D1BB80-F449-4442-8AAB-F71CF7F38B12}"/>
   </bookViews>
@@ -80,9 +80,6 @@
     <t>Detalles:</t>
   </si>
   <si>
-    <t>Piso :</t>
-  </si>
-  <si>
     <t>Area:</t>
   </si>
   <si>
@@ -315,6 +312,9 @@
   </si>
   <si>
     <t>Ing. Aguirre Alanya Luis Antonio CIP: 323997 CIV: 022178VCZRIX</t>
+  </si>
+  <si>
+    <t>Pisos:</t>
   </si>
 </sst>
 </file>
@@ -804,198 +804,163 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -1026,16 +991,16 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1065,118 +1030,153 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2169,86 +2169,86 @@
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="141" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
+      <c r="E4" s="141"/>
+      <c r="F4" s="141"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="142" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
+      <c r="E5" s="142"/>
+      <c r="F5" s="142"/>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="D6" s="143" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
+      <c r="E6" s="143"/>
+      <c r="F6" s="143"/>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="144" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
+      <c r="E7" s="144"/>
+      <c r="F7" s="144"/>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="46"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
+      <c r="A8" s="145"/>
+      <c r="B8" s="145"/>
+      <c r="C8" s="145"/>
+      <c r="D8" s="145"/>
+      <c r="E8" s="145"/>
+      <c r="F8" s="145"/>
+      <c r="G8" s="145"/>
+      <c r="H8" s="145"/>
     </row>
     <row r="9" spans="1:8" s="5" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="140" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
+      <c r="C9" s="140"/>
+      <c r="D9" s="140"/>
+      <c r="E9" s="140"/>
+      <c r="F9" s="140"/>
+      <c r="G9" s="140"/>
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:8" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
+      <c r="B10" s="140"/>
+      <c r="C10" s="140"/>
+      <c r="D10" s="140"/>
+      <c r="E10" s="140"/>
+      <c r="F10" s="140"/>
+      <c r="G10" s="140"/>
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="128" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
+      <c r="C11" s="128"/>
+      <c r="D11" s="128"/>
+      <c r="E11" s="128"/>
       <c r="F11" s="8" t="s">
         <v>12</v>
       </c>
@@ -2257,80 +2257,80 @@
     </row>
     <row r="12" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
+      <c r="B12" s="128"/>
+      <c r="C12" s="128"/>
+      <c r="D12" s="128"/>
+      <c r="E12" s="128"/>
+      <c r="F12" s="128"/>
+      <c r="G12" s="128"/>
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
+      <c r="B13" s="128"/>
+      <c r="C13" s="128"/>
+      <c r="D13" s="128"/>
+      <c r="E13" s="128"/>
+      <c r="F13" s="128"/>
+      <c r="G13" s="128"/>
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>13</v>
+        <v>91</v>
       </c>
       <c r="B14" s="40"/>
       <c r="C14" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="13" t="s">
         <v>15</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>16</v>
       </c>
       <c r="G14" s="16"/>
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="128"/>
+      <c r="C15" s="128"/>
+      <c r="D15" s="128"/>
+      <c r="E15" s="128"/>
+      <c r="F15" s="13" t="s">
         <v>17</v>
-      </c>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="13" t="s">
-        <v>18</v>
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
-      <c r="B16" s="51"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="51"/>
+      <c r="B16" s="129"/>
+      <c r="C16" s="129"/>
+      <c r="D16" s="129"/>
+      <c r="E16" s="129"/>
       <c r="F16" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G16" s="17"/>
       <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="128"/>
+      <c r="C17" s="128"/>
+      <c r="D17" s="18" t="s">
         <v>20</v>
-      </c>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="18" t="s">
-        <v>21</v>
       </c>
       <c r="E17" s="19">
         <f ca="1">TODAY()</f>
-        <v>45838</v>
+        <v>45842</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
@@ -2338,185 +2338,185 @@
     </row>
     <row r="18" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
-      <c r="B18" s="52"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="52"/>
+      <c r="B18" s="130"/>
+      <c r="C18" s="130"/>
+      <c r="D18" s="130"/>
+      <c r="E18" s="130"/>
+      <c r="F18" s="130"/>
+      <c r="G18" s="130"/>
       <c r="H18" s="20"/>
     </row>
     <row r="19" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
-      <c r="B19" s="53" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="54"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="56"/>
+      <c r="B19" s="131" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="132"/>
+      <c r="D19" s="133"/>
+      <c r="E19" s="134"/>
+      <c r="F19" s="134"/>
+      <c r="G19" s="134"/>
       <c r="H19" s="22"/>
     </row>
     <row r="20" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
-      <c r="B20" s="57" t="s">
+      <c r="B20" s="135" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="136"/>
+      <c r="D20" s="137"/>
+      <c r="E20" s="138" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="58"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="60" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20" s="60"/>
-      <c r="G20" s="61"/>
+      <c r="F20" s="138"/>
+      <c r="G20" s="139"/>
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="68" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="69"/>
+      <c r="D21" s="70"/>
+      <c r="E21" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="48" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" s="48"/>
-      <c r="G21" s="49"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="70"/>
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
-      <c r="B22" s="62" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="64"/>
-      <c r="G22" s="65"/>
+      <c r="B22" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="126"/>
+      <c r="F22" s="126"/>
+      <c r="G22" s="127"/>
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="68" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="69"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="48"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="F23" s="48"/>
-      <c r="G23" s="49"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="70"/>
       <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
-      <c r="B24" s="47" t="s">
+      <c r="B24" s="68" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="69"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="48"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="F24" s="48"/>
-      <c r="G24" s="49"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="70"/>
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="24"/>
-      <c r="B25" s="47" t="s">
+      <c r="B25" s="68" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="69"/>
+      <c r="D25" s="70"/>
+      <c r="E25" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="48"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="F25" s="48"/>
-      <c r="G25" s="49"/>
+      <c r="F25" s="69"/>
+      <c r="G25" s="70"/>
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="25"/>
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="69"/>
+      <c r="D26" s="70"/>
+      <c r="E26" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="48"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="F26" s="48"/>
-      <c r="G26" s="49"/>
+      <c r="F26" s="69"/>
+      <c r="G26" s="70"/>
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="25"/>
-      <c r="B27" s="69" t="s">
+      <c r="B27" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="53"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="70"/>
-      <c r="D27" s="71"/>
-      <c r="E27" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="F27" s="48"/>
-      <c r="G27" s="49"/>
+      <c r="F27" s="69"/>
+      <c r="G27" s="70"/>
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="25"/>
-      <c r="B28" s="72" t="s">
+      <c r="B28" s="112" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="113"/>
+      <c r="D28" s="114"/>
+      <c r="E28" s="115" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="73"/>
-      <c r="D28" s="74"/>
-      <c r="E28" s="75" t="s">
-        <v>39</v>
-      </c>
-      <c r="F28" s="76"/>
-      <c r="G28" s="77"/>
+      <c r="F28" s="116"/>
+      <c r="G28" s="117"/>
       <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="25"/>
-      <c r="B29" s="62" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="63"/>
-      <c r="D29" s="63"/>
-      <c r="E29" s="78"/>
-      <c r="F29" s="78"/>
-      <c r="G29" s="79"/>
+      <c r="B29" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="59"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="118"/>
+      <c r="F29" s="118"/>
+      <c r="G29" s="119"/>
       <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="26"/>
-      <c r="B30" s="80" t="s">
+      <c r="B30" s="120" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="121"/>
+      <c r="D30" s="122"/>
+      <c r="E30" s="123" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="81"/>
-      <c r="D30" s="82"/>
-      <c r="E30" s="83" t="s">
-        <v>42</v>
-      </c>
-      <c r="F30" s="84"/>
-      <c r="G30" s="85"/>
+      <c r="F30" s="124"/>
+      <c r="G30" s="125"/>
       <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="26"/>
-      <c r="B31" s="66" t="s">
+      <c r="B31" s="94" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="95"/>
+      <c r="D31" s="96"/>
+      <c r="E31" s="27" t="s">
         <v>43</v>
-      </c>
-      <c r="C31" s="67"/>
-      <c r="D31" s="68"/>
-      <c r="E31" s="27" t="s">
-        <v>44</v>
       </c>
       <c r="F31" s="28"/>
       <c r="G31" s="29"/>
@@ -2524,13 +2524,13 @@
     </row>
     <row r="32" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="30"/>
-      <c r="B32" s="86" t="s">
+      <c r="B32" s="106" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="107"/>
+      <c r="D32" s="108"/>
+      <c r="E32" s="27" t="s">
         <v>45</v>
-      </c>
-      <c r="C32" s="87"/>
-      <c r="D32" s="88"/>
-      <c r="E32" s="27" t="s">
-        <v>46</v>
       </c>
       <c r="F32" s="28"/>
       <c r="G32" s="29"/>
@@ -2538,308 +2538,308 @@
     </row>
     <row r="33" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
-      <c r="B33" s="86"/>
-      <c r="C33" s="87"/>
-      <c r="D33" s="88"/>
-      <c r="E33" s="69" t="s">
-        <v>47</v>
-      </c>
-      <c r="F33" s="70"/>
-      <c r="G33" s="71"/>
+      <c r="B33" s="106"/>
+      <c r="C33" s="107"/>
+      <c r="D33" s="108"/>
+      <c r="E33" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="F33" s="53"/>
+      <c r="G33" s="54"/>
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
-      <c r="B34" s="69" t="s">
+      <c r="B34" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" s="53"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="70"/>
-      <c r="D34" s="71"/>
-      <c r="E34" s="69" t="s">
-        <v>49</v>
-      </c>
-      <c r="F34" s="70"/>
-      <c r="G34" s="71"/>
+      <c r="F34" s="53"/>
+      <c r="G34" s="54"/>
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
-      <c r="B35" s="89" t="s">
+      <c r="B35" s="109" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="110"/>
+      <c r="D35" s="111"/>
+      <c r="E35" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="90"/>
-      <c r="D35" s="91"/>
-      <c r="E35" s="69" t="s">
-        <v>51</v>
-      </c>
-      <c r="F35" s="70"/>
-      <c r="G35" s="71"/>
+      <c r="F35" s="53"/>
+      <c r="G35" s="54"/>
       <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
-      <c r="B36" s="89"/>
-      <c r="C36" s="90"/>
-      <c r="D36" s="91"/>
-      <c r="E36" s="92" t="s">
-        <v>52</v>
-      </c>
-      <c r="F36" s="70"/>
-      <c r="G36" s="71"/>
+      <c r="B36" s="109"/>
+      <c r="C36" s="110"/>
+      <c r="D36" s="111"/>
+      <c r="E36" s="74" t="s">
+        <v>51</v>
+      </c>
+      <c r="F36" s="53"/>
+      <c r="G36" s="54"/>
       <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
-      <c r="B37" s="96" t="s">
+      <c r="B37" s="88" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="89"/>
+      <c r="D37" s="90"/>
+      <c r="E37" s="91" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="97"/>
-      <c r="D37" s="98"/>
-      <c r="E37" s="99" t="s">
-        <v>54</v>
-      </c>
-      <c r="F37" s="100"/>
-      <c r="G37" s="101"/>
+      <c r="F37" s="92"/>
+      <c r="G37" s="93"/>
       <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
-      <c r="B38" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="C38" s="67"/>
-      <c r="D38" s="68"/>
-      <c r="E38" s="99"/>
-      <c r="F38" s="100"/>
-      <c r="G38" s="101"/>
+      <c r="B38" s="94" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="95"/>
+      <c r="D38" s="96"/>
+      <c r="E38" s="91"/>
+      <c r="F38" s="92"/>
+      <c r="G38" s="93"/>
       <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
-      <c r="B39" s="102" t="s">
+      <c r="B39" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" s="66"/>
+      <c r="D39" s="67"/>
+      <c r="E39" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="103"/>
-      <c r="D39" s="104"/>
-      <c r="E39" s="105" t="s">
-        <v>57</v>
-      </c>
-      <c r="F39" s="106"/>
-      <c r="G39" s="107"/>
+      <c r="F39" s="98"/>
+      <c r="G39" s="99"/>
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
-      <c r="B40" s="102"/>
-      <c r="C40" s="103"/>
-      <c r="D40" s="104"/>
-      <c r="E40" s="108" t="s">
-        <v>58</v>
-      </c>
-      <c r="F40" s="109"/>
-      <c r="G40" s="110"/>
+      <c r="B40" s="65"/>
+      <c r="C40" s="66"/>
+      <c r="D40" s="67"/>
+      <c r="E40" s="100" t="s">
+        <v>57</v>
+      </c>
+      <c r="F40" s="101"/>
+      <c r="G40" s="102"/>
       <c r="H40" s="10"/>
     </row>
     <row r="41" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
-      <c r="B41" s="69" t="s">
+      <c r="B41" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" s="53"/>
+      <c r="D41" s="54"/>
+      <c r="E41" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="C41" s="70"/>
-      <c r="D41" s="71"/>
-      <c r="E41" s="99" t="s">
-        <v>60</v>
-      </c>
-      <c r="F41" s="100"/>
-      <c r="G41" s="101"/>
+      <c r="F41" s="92"/>
+      <c r="G41" s="93"/>
       <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
-      <c r="B42" s="69" t="s">
-        <v>61</v>
-      </c>
-      <c r="C42" s="70"/>
-      <c r="D42" s="71"/>
-      <c r="E42" s="99"/>
-      <c r="F42" s="100"/>
-      <c r="G42" s="101"/>
+      <c r="B42" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" s="53"/>
+      <c r="D42" s="54"/>
+      <c r="E42" s="91"/>
+      <c r="F42" s="92"/>
+      <c r="G42" s="93"/>
       <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
-      <c r="B43" s="69" t="s">
+      <c r="B43" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="53"/>
+      <c r="D43" s="54"/>
+      <c r="E43" s="103" t="s">
         <v>62</v>
       </c>
-      <c r="C43" s="70"/>
-      <c r="D43" s="71"/>
-      <c r="E43" s="111" t="s">
-        <v>63</v>
-      </c>
-      <c r="F43" s="112"/>
-      <c r="G43" s="113"/>
+      <c r="F43" s="104"/>
+      <c r="G43" s="105"/>
       <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
-      <c r="B44" s="69" t="s">
-        <v>64</v>
-      </c>
-      <c r="C44" s="70"/>
-      <c r="D44" s="71"/>
-      <c r="E44" s="93"/>
-      <c r="F44" s="94"/>
-      <c r="G44" s="95"/>
+      <c r="B44" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44" s="53"/>
+      <c r="D44" s="54"/>
+      <c r="E44" s="85"/>
+      <c r="F44" s="86"/>
+      <c r="G44" s="87"/>
       <c r="H44" s="10"/>
     </row>
     <row r="45" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
-      <c r="B45" s="69" t="s">
+      <c r="B45" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" s="53"/>
+      <c r="D45" s="54"/>
+      <c r="E45" s="55"/>
+      <c r="F45" s="56"/>
+      <c r="G45" s="57"/>
+      <c r="H45" s="10"/>
+    </row>
+    <row r="46" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="C45" s="70"/>
-      <c r="D45" s="71"/>
-      <c r="E45" s="115"/>
-      <c r="F45" s="116"/>
-      <c r="G45" s="117"/>
-      <c r="H45" s="10"/>
-    </row>
-    <row r="46" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="62" t="s">
-        <v>66</v>
-      </c>
-      <c r="C46" s="63"/>
-      <c r="D46" s="63"/>
-      <c r="E46" s="118"/>
-      <c r="F46" s="118"/>
-      <c r="G46" s="119"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="59"/>
+      <c r="E46" s="60"/>
+      <c r="F46" s="60"/>
+      <c r="G46" s="61"/>
       <c r="H46" s="10"/>
     </row>
     <row r="47" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
-      <c r="B47" s="120" t="s">
+      <c r="B47" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="C47" s="63"/>
+      <c r="D47" s="64"/>
+      <c r="E47" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="C47" s="121"/>
-      <c r="D47" s="122"/>
-      <c r="E47" s="47" t="s">
-        <v>68</v>
-      </c>
-      <c r="F47" s="48"/>
-      <c r="G47" s="49"/>
+      <c r="F47" s="69"/>
+      <c r="G47" s="70"/>
       <c r="H47" s="10"/>
     </row>
     <row r="48" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
-      <c r="B48" s="102"/>
-      <c r="C48" s="103"/>
-      <c r="D48" s="104"/>
-      <c r="E48" s="123" t="s">
-        <v>69</v>
-      </c>
-      <c r="F48" s="124"/>
-      <c r="G48" s="125"/>
+      <c r="B48" s="65"/>
+      <c r="C48" s="66"/>
+      <c r="D48" s="67"/>
+      <c r="E48" s="71" t="s">
+        <v>68</v>
+      </c>
+      <c r="F48" s="72"/>
+      <c r="G48" s="73"/>
       <c r="H48" s="10"/>
     </row>
     <row r="49" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
-      <c r="B49" s="102"/>
-      <c r="C49" s="103"/>
-      <c r="D49" s="104"/>
-      <c r="E49" s="92" t="s">
-        <v>70</v>
-      </c>
-      <c r="F49" s="126"/>
-      <c r="G49" s="127"/>
+      <c r="B49" s="65"/>
+      <c r="C49" s="66"/>
+      <c r="D49" s="67"/>
+      <c r="E49" s="74" t="s">
+        <v>69</v>
+      </c>
+      <c r="F49" s="75"/>
+      <c r="G49" s="76"/>
       <c r="H49" s="10"/>
     </row>
     <row r="50" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>
-      <c r="B50" s="128" t="s">
-        <v>71</v>
-      </c>
-      <c r="C50" s="129"/>
-      <c r="D50" s="130"/>
-      <c r="E50" s="131"/>
-      <c r="F50" s="132"/>
-      <c r="G50" s="133"/>
+      <c r="B50" s="77" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="78"/>
+      <c r="D50" s="79"/>
+      <c r="E50" s="80"/>
+      <c r="F50" s="81"/>
+      <c r="G50" s="82"/>
       <c r="H50" s="10"/>
     </row>
     <row r="51" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
-      <c r="B51" s="134"/>
-      <c r="C51" s="134"/>
-      <c r="D51" s="134"/>
-      <c r="E51" s="134"/>
-      <c r="F51" s="134"/>
-      <c r="G51" s="134"/>
+      <c r="B51" s="83"/>
+      <c r="C51" s="83"/>
+      <c r="D51" s="83"/>
+      <c r="E51" s="83"/>
+      <c r="F51" s="83"/>
+      <c r="G51" s="83"/>
       <c r="H51" s="10"/>
     </row>
     <row r="52" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
       <c r="B52" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="C52" s="135"/>
-      <c r="D52" s="135"/>
-      <c r="E52" s="135"/>
-      <c r="F52" s="135"/>
-      <c r="G52" s="135"/>
+        <v>71</v>
+      </c>
+      <c r="C52" s="84"/>
+      <c r="D52" s="84"/>
+      <c r="E52" s="84"/>
+      <c r="F52" s="84"/>
+      <c r="G52" s="84"/>
       <c r="H52" s="10"/>
     </row>
     <row r="53" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
-      <c r="B53" s="114"/>
-      <c r="C53" s="114"/>
-      <c r="D53" s="114"/>
-      <c r="E53" s="114"/>
-      <c r="F53" s="114"/>
-      <c r="G53" s="114"/>
+      <c r="B53" s="51"/>
+      <c r="C53" s="51"/>
+      <c r="D53" s="51"/>
+      <c r="E53" s="51"/>
+      <c r="F53" s="51"/>
+      <c r="G53" s="51"/>
       <c r="H53" s="10"/>
     </row>
     <row r="54" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
-      <c r="B54" s="114"/>
-      <c r="C54" s="114"/>
-      <c r="D54" s="114"/>
-      <c r="E54" s="114"/>
-      <c r="F54" s="114"/>
-      <c r="G54" s="114"/>
+      <c r="B54" s="51"/>
+      <c r="C54" s="51"/>
+      <c r="D54" s="51"/>
+      <c r="E54" s="51"/>
+      <c r="F54" s="51"/>
+      <c r="G54" s="51"/>
       <c r="H54" s="10"/>
     </row>
     <row r="55" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
-      <c r="B55" s="136"/>
-      <c r="C55" s="136"/>
-      <c r="D55" s="136"/>
-      <c r="E55" s="136"/>
-      <c r="F55" s="136"/>
-      <c r="G55" s="136"/>
+      <c r="B55" s="47"/>
+      <c r="C55" s="47"/>
+      <c r="D55" s="47"/>
+      <c r="E55" s="47"/>
+      <c r="F55" s="47"/>
+      <c r="G55" s="47"/>
       <c r="H55" s="10"/>
     </row>
     <row r="56" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="21"/>
-      <c r="B56" s="137" t="s">
-        <v>73</v>
-      </c>
-      <c r="C56" s="137"/>
-      <c r="D56" s="137"/>
-      <c r="E56" s="137"/>
-      <c r="F56" s="137"/>
-      <c r="G56" s="137"/>
+      <c r="B56" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="C56" s="43"/>
+      <c r="D56" s="43"/>
+      <c r="E56" s="43"/>
+      <c r="F56" s="43"/>
+      <c r="G56" s="43"/>
       <c r="H56" s="22"/>
     </row>
     <row r="57" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="22"/>
-      <c r="B57" s="138" t="s">
-        <v>74</v>
-      </c>
-      <c r="C57" s="138"/>
+      <c r="B57" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="C57" s="48"/>
       <c r="D57" s="32">
         <v>7</v>
       </c>
       <c r="E57" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F57" s="20"/>
       <c r="G57" s="20"/>
@@ -2847,135 +2847,135 @@
     </row>
     <row r="58" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="21"/>
-      <c r="B58" s="137" t="s">
-        <v>76</v>
-      </c>
-      <c r="C58" s="137"/>
-      <c r="D58" s="137"/>
-      <c r="E58" s="137"/>
-      <c r="F58" s="137"/>
-      <c r="G58" s="137"/>
+      <c r="B58" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="C58" s="43"/>
+      <c r="D58" s="43"/>
+      <c r="E58" s="43"/>
+      <c r="F58" s="43"/>
+      <c r="G58" s="43"/>
       <c r="H58" s="22"/>
     </row>
     <row r="59" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="22"/>
-      <c r="B59" s="139" t="s">
-        <v>77</v>
-      </c>
-      <c r="C59" s="139"/>
+      <c r="B59" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="C59" s="49"/>
       <c r="D59" s="33">
         <f>SUM(C61:C61)</f>
         <v>0</v>
       </c>
-      <c r="E59" s="140" t="s">
-        <v>78</v>
-      </c>
-      <c r="F59" s="140"/>
+      <c r="E59" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="F59" s="50"/>
       <c r="G59" s="20"/>
       <c r="H59" s="22"/>
     </row>
     <row r="60" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="21"/>
-      <c r="B60" s="137" t="s">
-        <v>79</v>
-      </c>
-      <c r="C60" s="137"/>
-      <c r="D60" s="137"/>
-      <c r="E60" s="137"/>
-      <c r="F60" s="137"/>
-      <c r="G60" s="137"/>
+      <c r="B60" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="C60" s="43"/>
+      <c r="D60" s="43"/>
+      <c r="E60" s="43"/>
+      <c r="F60" s="43"/>
+      <c r="G60" s="43"/>
       <c r="H60" s="22"/>
     </row>
     <row r="61" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="22"/>
       <c r="B61" s="34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C61" s="35"/>
-      <c r="D61" s="141" t="s">
-        <v>80</v>
-      </c>
-      <c r="E61" s="141"/>
-      <c r="F61" s="141"/>
+      <c r="D61" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="E61" s="44"/>
+      <c r="F61" s="44"/>
       <c r="G61" s="36">
         <f ca="1">E17</f>
-        <v>45838</v>
+        <v>45842</v>
       </c>
       <c r="H61" s="22"/>
     </row>
     <row r="62" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
-      <c r="B62" s="142" t="s">
-        <v>81</v>
-      </c>
-      <c r="C62" s="142"/>
-      <c r="D62" s="142"/>
-      <c r="E62" s="142"/>
-      <c r="F62" s="142"/>
-      <c r="G62" s="142"/>
+      <c r="B62" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="C62" s="45"/>
+      <c r="D62" s="45"/>
+      <c r="E62" s="45"/>
+      <c r="F62" s="45"/>
+      <c r="G62" s="45"/>
       <c r="H62" s="37"/>
     </row>
     <row r="63" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="B63" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="B63" s="143" t="s">
+      <c r="C63" s="46"/>
+      <c r="D63" s="46"/>
+      <c r="E63" s="46"/>
+      <c r="F63" s="46"/>
+      <c r="G63" s="46"/>
+    </row>
+    <row r="64" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="C64" s="42"/>
+      <c r="D64" s="42"/>
+      <c r="E64" s="42"/>
+      <c r="F64" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="C63" s="143"/>
-      <c r="D63" s="143"/>
-      <c r="E63" s="143"/>
-      <c r="F63" s="143"/>
-      <c r="G63" s="143"/>
-    </row>
-    <row r="64" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="144" t="s">
-        <v>91</v>
-      </c>
-      <c r="C64" s="144"/>
-      <c r="D64" s="144"/>
-      <c r="E64" s="144"/>
-      <c r="F64" s="144" t="s">
+      <c r="G64" s="42"/>
+      <c r="H64" s="42"/>
+    </row>
+    <row r="65" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="G64" s="144"/>
-      <c r="H64" s="144"/>
-    </row>
-    <row r="65" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="145" t="s">
+      <c r="C65" s="41"/>
+      <c r="D65" s="41"/>
+      <c r="E65" s="41"/>
+      <c r="F65" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="C65" s="145"/>
-      <c r="D65" s="145"/>
-      <c r="E65" s="145"/>
-      <c r="F65" s="144" t="s">
+      <c r="G65" s="42"/>
+      <c r="H65" s="42"/>
+    </row>
+    <row r="66" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="G65" s="144"/>
-      <c r="H65" s="144"/>
-    </row>
-    <row r="66" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="145" t="s">
+      <c r="C66" s="41"/>
+      <c r="D66" s="41"/>
+      <c r="E66" s="41"/>
+      <c r="F66" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="C66" s="145"/>
-      <c r="D66" s="145"/>
-      <c r="E66" s="145"/>
-      <c r="F66" s="144" t="s">
+      <c r="G66" s="42"/>
+      <c r="H66" s="42"/>
+    </row>
+    <row r="67" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="42" t="s">
         <v>88</v>
       </c>
-      <c r="G66" s="144"/>
-      <c r="H66" s="144"/>
-    </row>
-    <row r="67" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="144" t="s">
-        <v>89</v>
-      </c>
-      <c r="C67" s="144"/>
-      <c r="D67" s="144"/>
-      <c r="E67" s="144"/>
-      <c r="F67" s="144"/>
-      <c r="G67" s="144"/>
+      <c r="C67" s="42"/>
+      <c r="D67" s="42"/>
+      <c r="E67" s="42"/>
+      <c r="F67" s="42"/>
+      <c r="G67" s="42"/>
     </row>
     <row r="68" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="39"/>
@@ -3005,24 +3005,63 @@
     <protectedRange algorithmName="SHA-512" hashValue="1IwEtpPovyRjspz9ti3J5udl070IPZ9gDlGmM3ZH/lFyQlLVVL2qbaMds7kHvZZkPq7VvowLV2MqpNnf8owpjQ==" saltValue="SwYyjj//I75seGLqQP0hyQ==" spinCount="100000" sqref="E37:G38 E39" name="Rango2_2"/>
   </protectedRanges>
   <mergeCells count="88">
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="B66:E66"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="B62:G62"/>
-    <mergeCell ref="B63:G63"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="B55:G55"/>
-    <mergeCell ref="B56:G56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:G58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="B9:G10"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="B32:D33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="B35:D36"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:G38"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B39:D40"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="E41:G42"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="E43:G43"/>
     <mergeCell ref="B54:G54"/>
     <mergeCell ref="B45:D45"/>
     <mergeCell ref="E45:G45"/>
@@ -3036,63 +3075,24 @@
     <mergeCell ref="B51:G51"/>
     <mergeCell ref="C52:G52"/>
     <mergeCell ref="B53:G53"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E37:G38"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B39:D40"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="E41:G42"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="B32:D33"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="B35:D36"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="B9:G10"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="B56:G56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="B62:G62"/>
+    <mergeCell ref="B63:G63"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="B66:E66"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="F67:G67"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D7" r:id="rId1" xr:uid="{06F8AEE0-B467-46CC-BA80-3945E484B37D}"/>

</xml_diff>

<commit_message>
feat: se agrego la escarapela
</commit_message>
<xml_diff>
--- a/backend/docs/ACT-AUT.xlsx
+++ b/backend/docs/ACT-AUT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\planosperu-app\backend\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D2E014-5600-470F-B7E6-EC1170E9FF1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93731BE-B772-4A21-ADC3-6DBA28295A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{96D1BB80-F449-4442-8AAB-F71CF7F38B12}"/>
   </bookViews>
@@ -68,9 +68,6 @@
     <t>https://www.planosperu.com.pe</t>
   </si>
   <si>
-    <t>COTIZACION / CONTRATO DE TRAMITACIÓN DE ACTUALIZACIÓN DE TITULARIDAD DE AUTOVALUO - MUNICIPALIDAD</t>
-  </si>
-  <si>
     <t>Proyecto:</t>
   </si>
   <si>
@@ -315,6 +312,10 @@
   </si>
   <si>
     <t>Pisos:</t>
+  </si>
+  <si>
+    <t>COTIZACION / CONTRATO DE TRAMITACIÓN DE ACTUALIZACIÓN DE TITULARIDAD DE
+AUTOVALUO - MUNICIPALIDAD</t>
   </si>
 </sst>
 </file>
@@ -1840,6 +1841,56 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>285941</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>63792</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1644910-C08F-2487-4750-8224A33299DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5372100" y="657225"/>
+          <a:ext cx="838391" cy="1282992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2146,8 +2197,8 @@
   </sheetPr>
   <dimension ref="A3:H78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A60" zoomScale="130" zoomScaleNormal="50" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66:E66"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="50" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2221,7 +2272,7 @@
     </row>
     <row r="9" spans="1:8" s="5" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="140" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="C9" s="140"/>
       <c r="D9" s="140"/>
@@ -2241,16 +2292,16 @@
     </row>
     <row r="11" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="128" t="s">
         <v>10</v>
-      </c>
-      <c r="B11" s="128" t="s">
-        <v>11</v>
       </c>
       <c r="C11" s="128"/>
       <c r="D11" s="128"/>
       <c r="E11" s="128"/>
       <c r="F11" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="10"/>
@@ -2277,32 +2328,32 @@
     </row>
     <row r="14" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B14" s="40"/>
       <c r="C14" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="13" t="s">
         <v>14</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>15</v>
       </c>
       <c r="G14" s="16"/>
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="128"/>
       <c r="C15" s="128"/>
       <c r="D15" s="128"/>
       <c r="E15" s="128"/>
       <c r="F15" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="10"/>
@@ -2314,23 +2365,23 @@
       <c r="D16" s="129"/>
       <c r="E16" s="129"/>
       <c r="F16" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G16" s="17"/>
       <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="128"/>
       <c r="C17" s="128"/>
       <c r="D17" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17" s="19">
         <f ca="1">TODAY()</f>
-        <v>45842</v>
+        <v>45849</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
@@ -2349,7 +2400,7 @@
     <row r="19" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
       <c r="B19" s="131" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" s="132"/>
       <c r="D19" s="133"/>
@@ -2361,12 +2412,12 @@
     <row r="20" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="135" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" s="136"/>
       <c r="D20" s="137"/>
       <c r="E20" s="138" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F20" s="138"/>
       <c r="G20" s="139"/>
@@ -2375,12 +2426,12 @@
     <row r="21" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="68" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="69"/>
       <c r="D21" s="70"/>
       <c r="E21" s="69" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F21" s="69"/>
       <c r="G21" s="70"/>
@@ -2389,7 +2440,7 @@
     <row r="22" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="58" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" s="59"/>
       <c r="D22" s="59"/>
@@ -2401,12 +2452,12 @@
     <row r="23" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="68" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" s="69"/>
       <c r="D23" s="70"/>
       <c r="E23" s="68" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F23" s="69"/>
       <c r="G23" s="70"/>
@@ -2415,12 +2466,12 @@
     <row r="24" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="68" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" s="69"/>
       <c r="D24" s="70"/>
       <c r="E24" s="68" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F24" s="69"/>
       <c r="G24" s="70"/>
@@ -2429,12 +2480,12 @@
     <row r="25" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="24"/>
       <c r="B25" s="68" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25" s="69"/>
       <c r="D25" s="70"/>
       <c r="E25" s="68" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F25" s="69"/>
       <c r="G25" s="70"/>
@@ -2443,12 +2494,12 @@
     <row r="26" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="25"/>
       <c r="B26" s="68" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C26" s="69"/>
       <c r="D26" s="70"/>
       <c r="E26" s="68" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F26" s="69"/>
       <c r="G26" s="70"/>
@@ -2457,12 +2508,12 @@
     <row r="27" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="25"/>
       <c r="B27" s="52" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27" s="53"/>
       <c r="D27" s="54"/>
       <c r="E27" s="68" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F27" s="69"/>
       <c r="G27" s="70"/>
@@ -2471,12 +2522,12 @@
     <row r="28" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="25"/>
       <c r="B28" s="112" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C28" s="113"/>
       <c r="D28" s="114"/>
       <c r="E28" s="115" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F28" s="116"/>
       <c r="G28" s="117"/>
@@ -2485,7 +2536,7 @@
     <row r="29" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="25"/>
       <c r="B29" s="58" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C29" s="59"/>
       <c r="D29" s="59"/>
@@ -2497,12 +2548,12 @@
     <row r="30" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="26"/>
       <c r="B30" s="120" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C30" s="121"/>
       <c r="D30" s="122"/>
       <c r="E30" s="123" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F30" s="124"/>
       <c r="G30" s="125"/>
@@ -2511,12 +2562,12 @@
     <row r="31" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="26"/>
       <c r="B31" s="94" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C31" s="95"/>
       <c r="D31" s="96"/>
       <c r="E31" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F31" s="28"/>
       <c r="G31" s="29"/>
@@ -2525,12 +2576,12 @@
     <row r="32" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="30"/>
       <c r="B32" s="106" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C32" s="107"/>
       <c r="D32" s="108"/>
       <c r="E32" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F32" s="28"/>
       <c r="G32" s="29"/>
@@ -2542,7 +2593,7 @@
       <c r="C33" s="107"/>
       <c r="D33" s="108"/>
       <c r="E33" s="52" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F33" s="53"/>
       <c r="G33" s="54"/>
@@ -2551,12 +2602,12 @@
     <row r="34" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
       <c r="B34" s="52" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C34" s="53"/>
       <c r="D34" s="54"/>
       <c r="E34" s="52" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F34" s="53"/>
       <c r="G34" s="54"/>
@@ -2565,12 +2616,12 @@
     <row r="35" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
       <c r="B35" s="109" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C35" s="110"/>
       <c r="D35" s="111"/>
       <c r="E35" s="52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F35" s="53"/>
       <c r="G35" s="54"/>
@@ -2582,7 +2633,7 @@
       <c r="C36" s="110"/>
       <c r="D36" s="111"/>
       <c r="E36" s="74" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F36" s="53"/>
       <c r="G36" s="54"/>
@@ -2591,12 +2642,12 @@
     <row r="37" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
       <c r="B37" s="88" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C37" s="89"/>
       <c r="D37" s="90"/>
       <c r="E37" s="91" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F37" s="92"/>
       <c r="G37" s="93"/>
@@ -2605,7 +2656,7 @@
     <row r="38" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
       <c r="B38" s="94" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C38" s="95"/>
       <c r="D38" s="96"/>
@@ -2617,12 +2668,12 @@
     <row r="39" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
       <c r="B39" s="65" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C39" s="66"/>
       <c r="D39" s="67"/>
       <c r="E39" s="97" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F39" s="98"/>
       <c r="G39" s="99"/>
@@ -2634,7 +2685,7 @@
       <c r="C40" s="66"/>
       <c r="D40" s="67"/>
       <c r="E40" s="100" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F40" s="101"/>
       <c r="G40" s="102"/>
@@ -2643,12 +2694,12 @@
     <row r="41" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C41" s="53"/>
       <c r="D41" s="54"/>
       <c r="E41" s="91" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F41" s="92"/>
       <c r="G41" s="93"/>
@@ -2657,7 +2708,7 @@
     <row r="42" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="52" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C42" s="53"/>
       <c r="D42" s="54"/>
@@ -2669,12 +2720,12 @@
     <row r="43" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="B43" s="52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C43" s="53"/>
       <c r="D43" s="54"/>
       <c r="E43" s="103" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F43" s="104"/>
       <c r="G43" s="105"/>
@@ -2683,7 +2734,7 @@
     <row r="44" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C44" s="53"/>
       <c r="D44" s="54"/>
@@ -2695,7 +2746,7 @@
     <row r="45" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C45" s="53"/>
       <c r="D45" s="54"/>
@@ -2706,7 +2757,7 @@
     </row>
     <row r="46" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="58" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C46" s="59"/>
       <c r="D46" s="59"/>
@@ -2718,12 +2769,12 @@
     <row r="47" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="62" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C47" s="63"/>
       <c r="D47" s="64"/>
       <c r="E47" s="68" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F47" s="69"/>
       <c r="G47" s="70"/>
@@ -2735,7 +2786,7 @@
       <c r="C48" s="66"/>
       <c r="D48" s="67"/>
       <c r="E48" s="71" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F48" s="72"/>
       <c r="G48" s="73"/>
@@ -2747,7 +2798,7 @@
       <c r="C49" s="66"/>
       <c r="D49" s="67"/>
       <c r="E49" s="74" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F49" s="75"/>
       <c r="G49" s="76"/>
@@ -2756,7 +2807,7 @@
     <row r="50" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>
       <c r="B50" s="77" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C50" s="78"/>
       <c r="D50" s="79"/>
@@ -2778,7 +2829,7 @@
     <row r="52" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
       <c r="B52" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C52" s="84"/>
       <c r="D52" s="84"/>
@@ -2820,7 +2871,7 @@
     <row r="56" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="21"/>
       <c r="B56" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C56" s="43"/>
       <c r="D56" s="43"/>
@@ -2832,14 +2883,14 @@
     <row r="57" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="22"/>
       <c r="B57" s="48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C57" s="48"/>
       <c r="D57" s="32">
         <v>7</v>
       </c>
       <c r="E57" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F57" s="20"/>
       <c r="G57" s="20"/>
@@ -2848,7 +2899,7 @@
     <row r="58" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="21"/>
       <c r="B58" s="43" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C58" s="43"/>
       <c r="D58" s="43"/>
@@ -2860,7 +2911,7 @@
     <row r="59" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="22"/>
       <c r="B59" s="49" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C59" s="49"/>
       <c r="D59" s="33">
@@ -2868,7 +2919,7 @@
         <v>0</v>
       </c>
       <c r="E59" s="50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F59" s="50"/>
       <c r="G59" s="20"/>
@@ -2877,7 +2928,7 @@
     <row r="60" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="21"/>
       <c r="B60" s="43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C60" s="43"/>
       <c r="D60" s="43"/>
@@ -2889,24 +2940,24 @@
     <row r="61" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="22"/>
       <c r="B61" s="34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C61" s="35"/>
       <c r="D61" s="44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E61" s="44"/>
       <c r="F61" s="44"/>
       <c r="G61" s="36">
         <f ca="1">E17</f>
-        <v>45842</v>
+        <v>45849</v>
       </c>
       <c r="H61" s="22"/>
     </row>
     <row r="62" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
       <c r="B62" s="45" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C62" s="45"/>
       <c r="D62" s="45"/>
@@ -2917,10 +2968,10 @@
     </row>
     <row r="63" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="B63" s="46" t="s">
         <v>81</v>
-      </c>
-      <c r="B63" s="46" t="s">
-        <v>82</v>
       </c>
       <c r="C63" s="46"/>
       <c r="D63" s="46"/>
@@ -2930,46 +2981,46 @@
     </row>
     <row r="64" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C64" s="42"/>
       <c r="D64" s="42"/>
       <c r="E64" s="42"/>
       <c r="F64" s="42" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G64" s="42"/>
       <c r="H64" s="42"/>
     </row>
     <row r="65" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C65" s="41"/>
       <c r="D65" s="41"/>
       <c r="E65" s="41"/>
       <c r="F65" s="42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G65" s="42"/>
       <c r="H65" s="42"/>
     </row>
     <row r="66" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C66" s="41"/>
       <c r="D66" s="41"/>
       <c r="E66" s="41"/>
       <c r="F66" s="42" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G66" s="42"/>
       <c r="H66" s="42"/>
     </row>
     <row r="67" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C67" s="42"/>
       <c r="D67" s="42"/>

</xml_diff>

<commit_message>
feat: quitado las escarapelas
</commit_message>
<xml_diff>
--- a/backend/docs/ACT-AUT.xlsx
+++ b/backend/docs/ACT-AUT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\planosperu-app\backend\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Documents\planosperu-app\backend\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93731BE-B772-4A21-ADC3-6DBA28295A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC76CBF-ACDC-4B52-B7E5-9D0A230F0F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{96D1BB80-F449-4442-8AAB-F71CF7F38B12}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{96D1BB80-F449-4442-8AAB-F71CF7F38B12}"/>
   </bookViews>
   <sheets>
     <sheet name="ACT-AUT" sheetId="2" r:id="rId1"/>
@@ -805,42 +805,104 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -854,114 +916,87 @@
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -992,16 +1027,16 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1031,153 +1066,118 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1841,56 +1841,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>285941</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>63792</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1644910-C08F-2487-4750-8224A33299DF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5372100" y="657225"/>
-          <a:ext cx="838391" cy="1282992"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2220,86 +2170,86 @@
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="141" t="s">
+      <c r="D4" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="141"/>
-      <c r="F4" s="141"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="142" t="s">
+      <c r="D5" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="142"/>
-      <c r="F5" s="142"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="143" t="s">
+      <c r="D6" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="143"/>
-      <c r="F6" s="143"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="144" t="s">
+      <c r="D7" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="144"/>
-      <c r="F7" s="144"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="145"/>
-      <c r="B8" s="145"/>
-      <c r="C8" s="145"/>
-      <c r="D8" s="145"/>
-      <c r="E8" s="145"/>
-      <c r="F8" s="145"/>
-      <c r="G8" s="145"/>
-      <c r="H8" s="145"/>
+      <c r="A8" s="46"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
     </row>
     <row r="9" spans="1:8" s="5" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="140" t="s">
+      <c r="B9" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="140"/>
-      <c r="D9" s="140"/>
-      <c r="E9" s="140"/>
-      <c r="F9" s="140"/>
-      <c r="G9" s="140"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:8" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="140"/>
-      <c r="C10" s="140"/>
-      <c r="D10" s="140"/>
-      <c r="E10" s="140"/>
-      <c r="F10" s="140"/>
-      <c r="G10" s="140"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="128" t="s">
+      <c r="B11" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="128"/>
-      <c r="D11" s="128"/>
-      <c r="E11" s="128"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
       <c r="F11" s="8" t="s">
         <v>11</v>
       </c>
@@ -2308,22 +2258,22 @@
     </row>
     <row r="12" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="128"/>
-      <c r="C12" s="128"/>
-      <c r="D12" s="128"/>
-      <c r="E12" s="128"/>
-      <c r="F12" s="128"/>
-      <c r="G12" s="128"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
-      <c r="B13" s="128"/>
-      <c r="C13" s="128"/>
-      <c r="D13" s="128"/>
-      <c r="E13" s="128"/>
-      <c r="F13" s="128"/>
-      <c r="G13" s="128"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -2348,10 +2298,10 @@
       <c r="A15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="128"/>
-      <c r="C15" s="128"/>
-      <c r="D15" s="128"/>
-      <c r="E15" s="128"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
       <c r="F15" s="13" t="s">
         <v>16</v>
       </c>
@@ -2360,10 +2310,10 @@
     </row>
     <row r="16" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
-      <c r="B16" s="129"/>
-      <c r="C16" s="129"/>
-      <c r="D16" s="129"/>
-      <c r="E16" s="129"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
       <c r="F16" s="13" t="s">
         <v>17</v>
       </c>
@@ -2374,14 +2324,14 @@
       <c r="A17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="128"/>
-      <c r="C17" s="128"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
       <c r="D17" s="18" t="s">
         <v>19</v>
       </c>
       <c r="E17" s="19">
         <f ca="1">TODAY()</f>
-        <v>45849</v>
+        <v>45870</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
@@ -2389,183 +2339,183 @@
     </row>
     <row r="18" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
-      <c r="B18" s="130"/>
-      <c r="C18" s="130"/>
-      <c r="D18" s="130"/>
-      <c r="E18" s="130"/>
-      <c r="F18" s="130"/>
-      <c r="G18" s="130"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
       <c r="H18" s="20"/>
     </row>
     <row r="19" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
-      <c r="B19" s="131" t="s">
+      <c r="B19" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="132"/>
-      <c r="D19" s="133"/>
-      <c r="E19" s="134"/>
-      <c r="F19" s="134"/>
-      <c r="G19" s="134"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="56"/>
       <c r="H19" s="22"/>
     </row>
     <row r="20" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
-      <c r="B20" s="135" t="s">
+      <c r="B20" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="136"/>
-      <c r="D20" s="137"/>
-      <c r="E20" s="138" t="s">
+      <c r="C20" s="58"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="138"/>
-      <c r="G20" s="139"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="61"/>
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
-      <c r="B21" s="68" t="s">
+      <c r="B21" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="69"/>
-      <c r="D21" s="70"/>
-      <c r="E21" s="69" t="s">
+      <c r="C21" s="48"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="69"/>
-      <c r="G21" s="70"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="49"/>
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
-      <c r="B22" s="58" t="s">
+      <c r="B22" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="59"/>
-      <c r="D22" s="59"/>
-      <c r="E22" s="126"/>
-      <c r="F22" s="126"/>
-      <c r="G22" s="127"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="65"/>
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
-      <c r="B23" s="68" t="s">
+      <c r="B23" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="69"/>
-      <c r="D23" s="70"/>
-      <c r="E23" s="68" t="s">
+      <c r="C23" s="48"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="69"/>
-      <c r="G23" s="70"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="49"/>
       <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
-      <c r="B24" s="68" t="s">
+      <c r="B24" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="69"/>
-      <c r="D24" s="70"/>
-      <c r="E24" s="68" t="s">
+      <c r="C24" s="48"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="F24" s="69"/>
-      <c r="G24" s="70"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="49"/>
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="24"/>
-      <c r="B25" s="68" t="s">
+      <c r="B25" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="69"/>
-      <c r="D25" s="70"/>
-      <c r="E25" s="68" t="s">
+      <c r="C25" s="48"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="F25" s="69"/>
-      <c r="G25" s="70"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="49"/>
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="25"/>
-      <c r="B26" s="68" t="s">
+      <c r="B26" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="69"/>
-      <c r="D26" s="70"/>
-      <c r="E26" s="68" t="s">
+      <c r="C26" s="48"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="69"/>
-      <c r="G26" s="70"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="49"/>
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="25"/>
-      <c r="B27" s="52" t="s">
+      <c r="B27" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="53"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="68" t="s">
+      <c r="C27" s="70"/>
+      <c r="D27" s="71"/>
+      <c r="E27" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="F27" s="69"/>
-      <c r="G27" s="70"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="49"/>
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="25"/>
-      <c r="B28" s="112" t="s">
+      <c r="B28" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="113"/>
-      <c r="D28" s="114"/>
-      <c r="E28" s="115" t="s">
+      <c r="C28" s="73"/>
+      <c r="D28" s="74"/>
+      <c r="E28" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="F28" s="116"/>
-      <c r="G28" s="117"/>
+      <c r="F28" s="76"/>
+      <c r="G28" s="77"/>
       <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="25"/>
-      <c r="B29" s="58" t="s">
+      <c r="B29" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="59"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="118"/>
-      <c r="F29" s="118"/>
-      <c r="G29" s="119"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="78"/>
+      <c r="F29" s="78"/>
+      <c r="G29" s="79"/>
       <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="26"/>
-      <c r="B30" s="120" t="s">
+      <c r="B30" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="121"/>
-      <c r="D30" s="122"/>
-      <c r="E30" s="123" t="s">
+      <c r="C30" s="81"/>
+      <c r="D30" s="82"/>
+      <c r="E30" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="F30" s="124"/>
-      <c r="G30" s="125"/>
+      <c r="F30" s="84"/>
+      <c r="G30" s="85"/>
       <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="26"/>
-      <c r="B31" s="94" t="s">
+      <c r="B31" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="95"/>
-      <c r="D31" s="96"/>
+      <c r="C31" s="67"/>
+      <c r="D31" s="68"/>
       <c r="E31" s="27" t="s">
         <v>42</v>
       </c>
@@ -2575,11 +2525,11 @@
     </row>
     <row r="32" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="30"/>
-      <c r="B32" s="106" t="s">
+      <c r="B32" s="86" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="107"/>
-      <c r="D32" s="108"/>
+      <c r="C32" s="87"/>
+      <c r="D32" s="88"/>
       <c r="E32" s="27" t="s">
         <v>44</v>
       </c>
@@ -2589,241 +2539,241 @@
     </row>
     <row r="33" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
-      <c r="B33" s="106"/>
-      <c r="C33" s="107"/>
-      <c r="D33" s="108"/>
-      <c r="E33" s="52" t="s">
+      <c r="B33" s="86"/>
+      <c r="C33" s="87"/>
+      <c r="D33" s="88"/>
+      <c r="E33" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="F33" s="53"/>
-      <c r="G33" s="54"/>
+      <c r="F33" s="70"/>
+      <c r="G33" s="71"/>
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
-      <c r="B34" s="52" t="s">
+      <c r="B34" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="53"/>
-      <c r="D34" s="54"/>
-      <c r="E34" s="52" t="s">
+      <c r="C34" s="70"/>
+      <c r="D34" s="71"/>
+      <c r="E34" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="F34" s="53"/>
-      <c r="G34" s="54"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="71"/>
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
-      <c r="B35" s="109" t="s">
+      <c r="B35" s="89" t="s">
         <v>48</v>
       </c>
-      <c r="C35" s="110"/>
-      <c r="D35" s="111"/>
-      <c r="E35" s="52" t="s">
+      <c r="C35" s="90"/>
+      <c r="D35" s="91"/>
+      <c r="E35" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="F35" s="53"/>
-      <c r="G35" s="54"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="71"/>
       <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
-      <c r="B36" s="109"/>
-      <c r="C36" s="110"/>
-      <c r="D36" s="111"/>
-      <c r="E36" s="74" t="s">
+      <c r="B36" s="89"/>
+      <c r="C36" s="90"/>
+      <c r="D36" s="91"/>
+      <c r="E36" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="F36" s="53"/>
-      <c r="G36" s="54"/>
+      <c r="F36" s="70"/>
+      <c r="G36" s="71"/>
       <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
-      <c r="B37" s="88" t="s">
+      <c r="B37" s="96" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="89"/>
-      <c r="D37" s="90"/>
-      <c r="E37" s="91" t="s">
+      <c r="C37" s="97"/>
+      <c r="D37" s="98"/>
+      <c r="E37" s="99" t="s">
         <v>52</v>
       </c>
-      <c r="F37" s="92"/>
-      <c r="G37" s="93"/>
+      <c r="F37" s="100"/>
+      <c r="G37" s="101"/>
       <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
-      <c r="B38" s="94" t="s">
+      <c r="B38" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="C38" s="95"/>
-      <c r="D38" s="96"/>
-      <c r="E38" s="91"/>
-      <c r="F38" s="92"/>
-      <c r="G38" s="93"/>
+      <c r="C38" s="67"/>
+      <c r="D38" s="68"/>
+      <c r="E38" s="99"/>
+      <c r="F38" s="100"/>
+      <c r="G38" s="101"/>
       <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
-      <c r="B39" s="65" t="s">
+      <c r="B39" s="102" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="66"/>
-      <c r="D39" s="67"/>
-      <c r="E39" s="97" t="s">
+      <c r="C39" s="103"/>
+      <c r="D39" s="104"/>
+      <c r="E39" s="105" t="s">
         <v>55</v>
       </c>
-      <c r="F39" s="98"/>
-      <c r="G39" s="99"/>
+      <c r="F39" s="106"/>
+      <c r="G39" s="107"/>
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
-      <c r="B40" s="65"/>
-      <c r="C40" s="66"/>
-      <c r="D40" s="67"/>
-      <c r="E40" s="100" t="s">
+      <c r="B40" s="102"/>
+      <c r="C40" s="103"/>
+      <c r="D40" s="104"/>
+      <c r="E40" s="108" t="s">
         <v>56</v>
       </c>
-      <c r="F40" s="101"/>
-      <c r="G40" s="102"/>
+      <c r="F40" s="109"/>
+      <c r="G40" s="110"/>
       <c r="H40" s="10"/>
     </row>
     <row r="41" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
-      <c r="B41" s="52" t="s">
+      <c r="B41" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="53"/>
-      <c r="D41" s="54"/>
-      <c r="E41" s="91" t="s">
+      <c r="C41" s="70"/>
+      <c r="D41" s="71"/>
+      <c r="E41" s="99" t="s">
         <v>58</v>
       </c>
-      <c r="F41" s="92"/>
-      <c r="G41" s="93"/>
+      <c r="F41" s="100"/>
+      <c r="G41" s="101"/>
       <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
-      <c r="B42" s="52" t="s">
+      <c r="B42" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="C42" s="53"/>
-      <c r="D42" s="54"/>
-      <c r="E42" s="91"/>
-      <c r="F42" s="92"/>
-      <c r="G42" s="93"/>
+      <c r="C42" s="70"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="99"/>
+      <c r="F42" s="100"/>
+      <c r="G42" s="101"/>
       <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
-      <c r="B43" s="52" t="s">
+      <c r="B43" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="C43" s="53"/>
-      <c r="D43" s="54"/>
-      <c r="E43" s="103" t="s">
+      <c r="C43" s="70"/>
+      <c r="D43" s="71"/>
+      <c r="E43" s="111" t="s">
         <v>61</v>
       </c>
-      <c r="F43" s="104"/>
-      <c r="G43" s="105"/>
+      <c r="F43" s="112"/>
+      <c r="G43" s="113"/>
       <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
-      <c r="B44" s="52" t="s">
+      <c r="B44" s="69" t="s">
         <v>62</v>
       </c>
-      <c r="C44" s="53"/>
-      <c r="D44" s="54"/>
-      <c r="E44" s="85"/>
-      <c r="F44" s="86"/>
-      <c r="G44" s="87"/>
+      <c r="C44" s="70"/>
+      <c r="D44" s="71"/>
+      <c r="E44" s="93"/>
+      <c r="F44" s="94"/>
+      <c r="G44" s="95"/>
       <c r="H44" s="10"/>
     </row>
     <row r="45" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
-      <c r="B45" s="52" t="s">
+      <c r="B45" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="C45" s="53"/>
-      <c r="D45" s="54"/>
-      <c r="E45" s="55"/>
-      <c r="F45" s="56"/>
-      <c r="G45" s="57"/>
+      <c r="C45" s="70"/>
+      <c r="D45" s="71"/>
+      <c r="E45" s="115"/>
+      <c r="F45" s="116"/>
+      <c r="G45" s="117"/>
       <c r="H45" s="10"/>
     </row>
     <row r="46" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="58" t="s">
+      <c r="B46" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="59"/>
-      <c r="D46" s="59"/>
-      <c r="E46" s="60"/>
-      <c r="F46" s="60"/>
-      <c r="G46" s="61"/>
+      <c r="C46" s="63"/>
+      <c r="D46" s="63"/>
+      <c r="E46" s="118"/>
+      <c r="F46" s="118"/>
+      <c r="G46" s="119"/>
       <c r="H46" s="10"/>
     </row>
     <row r="47" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
-      <c r="B47" s="62" t="s">
+      <c r="B47" s="120" t="s">
         <v>65</v>
       </c>
-      <c r="C47" s="63"/>
-      <c r="D47" s="64"/>
-      <c r="E47" s="68" t="s">
+      <c r="C47" s="121"/>
+      <c r="D47" s="122"/>
+      <c r="E47" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="F47" s="69"/>
-      <c r="G47" s="70"/>
+      <c r="F47" s="48"/>
+      <c r="G47" s="49"/>
       <c r="H47" s="10"/>
     </row>
     <row r="48" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
-      <c r="B48" s="65"/>
-      <c r="C48" s="66"/>
-      <c r="D48" s="67"/>
-      <c r="E48" s="71" t="s">
+      <c r="B48" s="102"/>
+      <c r="C48" s="103"/>
+      <c r="D48" s="104"/>
+      <c r="E48" s="123" t="s">
         <v>67</v>
       </c>
-      <c r="F48" s="72"/>
-      <c r="G48" s="73"/>
+      <c r="F48" s="124"/>
+      <c r="G48" s="125"/>
       <c r="H48" s="10"/>
     </row>
     <row r="49" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
-      <c r="B49" s="65"/>
-      <c r="C49" s="66"/>
-      <c r="D49" s="67"/>
-      <c r="E49" s="74" t="s">
+      <c r="B49" s="102"/>
+      <c r="C49" s="103"/>
+      <c r="D49" s="104"/>
+      <c r="E49" s="92" t="s">
         <v>68</v>
       </c>
-      <c r="F49" s="75"/>
-      <c r="G49" s="76"/>
+      <c r="F49" s="126"/>
+      <c r="G49" s="127"/>
       <c r="H49" s="10"/>
     </row>
     <row r="50" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>
-      <c r="B50" s="77" t="s">
+      <c r="B50" s="128" t="s">
         <v>69</v>
       </c>
-      <c r="C50" s="78"/>
-      <c r="D50" s="79"/>
-      <c r="E50" s="80"/>
-      <c r="F50" s="81"/>
-      <c r="G50" s="82"/>
+      <c r="C50" s="129"/>
+      <c r="D50" s="130"/>
+      <c r="E50" s="131"/>
+      <c r="F50" s="132"/>
+      <c r="G50" s="133"/>
       <c r="H50" s="10"/>
     </row>
     <row r="51" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
-      <c r="B51" s="83"/>
-      <c r="C51" s="83"/>
-      <c r="D51" s="83"/>
-      <c r="E51" s="83"/>
-      <c r="F51" s="83"/>
-      <c r="G51" s="83"/>
+      <c r="B51" s="134"/>
+      <c r="C51" s="134"/>
+      <c r="D51" s="134"/>
+      <c r="E51" s="134"/>
+      <c r="F51" s="134"/>
+      <c r="G51" s="134"/>
       <c r="H51" s="10"/>
     </row>
     <row r="52" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -2831,61 +2781,61 @@
       <c r="B52" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="C52" s="84"/>
-      <c r="D52" s="84"/>
-      <c r="E52" s="84"/>
-      <c r="F52" s="84"/>
-      <c r="G52" s="84"/>
+      <c r="C52" s="135"/>
+      <c r="D52" s="135"/>
+      <c r="E52" s="135"/>
+      <c r="F52" s="135"/>
+      <c r="G52" s="135"/>
       <c r="H52" s="10"/>
     </row>
     <row r="53" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
-      <c r="B53" s="51"/>
-      <c r="C53" s="51"/>
-      <c r="D53" s="51"/>
-      <c r="E53" s="51"/>
-      <c r="F53" s="51"/>
-      <c r="G53" s="51"/>
+      <c r="B53" s="114"/>
+      <c r="C53" s="114"/>
+      <c r="D53" s="114"/>
+      <c r="E53" s="114"/>
+      <c r="F53" s="114"/>
+      <c r="G53" s="114"/>
       <c r="H53" s="10"/>
     </row>
     <row r="54" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
-      <c r="B54" s="51"/>
-      <c r="C54" s="51"/>
-      <c r="D54" s="51"/>
-      <c r="E54" s="51"/>
-      <c r="F54" s="51"/>
-      <c r="G54" s="51"/>
+      <c r="B54" s="114"/>
+      <c r="C54" s="114"/>
+      <c r="D54" s="114"/>
+      <c r="E54" s="114"/>
+      <c r="F54" s="114"/>
+      <c r="G54" s="114"/>
       <c r="H54" s="10"/>
     </row>
     <row r="55" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
-      <c r="B55" s="47"/>
-      <c r="C55" s="47"/>
-      <c r="D55" s="47"/>
-      <c r="E55" s="47"/>
-      <c r="F55" s="47"/>
-      <c r="G55" s="47"/>
+      <c r="B55" s="136"/>
+      <c r="C55" s="136"/>
+      <c r="D55" s="136"/>
+      <c r="E55" s="136"/>
+      <c r="F55" s="136"/>
+      <c r="G55" s="136"/>
       <c r="H55" s="10"/>
     </row>
     <row r="56" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="21"/>
-      <c r="B56" s="43" t="s">
+      <c r="B56" s="137" t="s">
         <v>71</v>
       </c>
-      <c r="C56" s="43"/>
-      <c r="D56" s="43"/>
-      <c r="E56" s="43"/>
-      <c r="F56" s="43"/>
-      <c r="G56" s="43"/>
+      <c r="C56" s="137"/>
+      <c r="D56" s="137"/>
+      <c r="E56" s="137"/>
+      <c r="F56" s="137"/>
+      <c r="G56" s="137"/>
       <c r="H56" s="22"/>
     </row>
     <row r="57" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="22"/>
-      <c r="B57" s="48" t="s">
+      <c r="B57" s="138" t="s">
         <v>72</v>
       </c>
-      <c r="C57" s="48"/>
+      <c r="C57" s="138"/>
       <c r="D57" s="32">
         <v>7</v>
       </c>
@@ -2898,43 +2848,43 @@
     </row>
     <row r="58" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="21"/>
-      <c r="B58" s="43" t="s">
+      <c r="B58" s="137" t="s">
         <v>74</v>
       </c>
-      <c r="C58" s="43"/>
-      <c r="D58" s="43"/>
-      <c r="E58" s="43"/>
-      <c r="F58" s="43"/>
-      <c r="G58" s="43"/>
+      <c r="C58" s="137"/>
+      <c r="D58" s="137"/>
+      <c r="E58" s="137"/>
+      <c r="F58" s="137"/>
+      <c r="G58" s="137"/>
       <c r="H58" s="22"/>
     </row>
     <row r="59" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="22"/>
-      <c r="B59" s="49" t="s">
+      <c r="B59" s="139" t="s">
         <v>75</v>
       </c>
-      <c r="C59" s="49"/>
+      <c r="C59" s="139"/>
       <c r="D59" s="33">
         <f>SUM(C61:C61)</f>
         <v>0</v>
       </c>
-      <c r="E59" s="50" t="s">
+      <c r="E59" s="140" t="s">
         <v>76</v>
       </c>
-      <c r="F59" s="50"/>
+      <c r="F59" s="140"/>
       <c r="G59" s="20"/>
       <c r="H59" s="22"/>
     </row>
     <row r="60" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="21"/>
-      <c r="B60" s="43" t="s">
+      <c r="B60" s="137" t="s">
         <v>77</v>
       </c>
-      <c r="C60" s="43"/>
-      <c r="D60" s="43"/>
-      <c r="E60" s="43"/>
-      <c r="F60" s="43"/>
-      <c r="G60" s="43"/>
+      <c r="C60" s="137"/>
+      <c r="D60" s="137"/>
+      <c r="E60" s="137"/>
+      <c r="F60" s="137"/>
+      <c r="G60" s="137"/>
       <c r="H60" s="22"/>
     </row>
     <row r="61" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -2943,90 +2893,90 @@
         <v>88</v>
       </c>
       <c r="C61" s="35"/>
-      <c r="D61" s="44" t="s">
+      <c r="D61" s="141" t="s">
         <v>78</v>
       </c>
-      <c r="E61" s="44"/>
-      <c r="F61" s="44"/>
+      <c r="E61" s="141"/>
+      <c r="F61" s="141"/>
       <c r="G61" s="36">
         <f ca="1">E17</f>
-        <v>45849</v>
+        <v>45870</v>
       </c>
       <c r="H61" s="22"/>
     </row>
     <row r="62" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
-      <c r="B62" s="45" t="s">
+      <c r="B62" s="142" t="s">
         <v>79</v>
       </c>
-      <c r="C62" s="45"/>
-      <c r="D62" s="45"/>
-      <c r="E62" s="45"/>
-      <c r="F62" s="45"/>
-      <c r="G62" s="45"/>
+      <c r="C62" s="142"/>
+      <c r="D62" s="142"/>
+      <c r="E62" s="142"/>
+      <c r="F62" s="142"/>
+      <c r="G62" s="142"/>
       <c r="H62" s="37"/>
     </row>
     <row r="63" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="B63" s="46" t="s">
+      <c r="B63" s="143" t="s">
         <v>81</v>
       </c>
-      <c r="C63" s="46"/>
-      <c r="D63" s="46"/>
-      <c r="E63" s="46"/>
-      <c r="F63" s="46"/>
-      <c r="G63" s="46"/>
+      <c r="C63" s="143"/>
+      <c r="D63" s="143"/>
+      <c r="E63" s="143"/>
+      <c r="F63" s="143"/>
+      <c r="G63" s="143"/>
     </row>
     <row r="64" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="42" t="s">
+      <c r="B64" s="144" t="s">
         <v>89</v>
       </c>
-      <c r="C64" s="42"/>
-      <c r="D64" s="42"/>
-      <c r="E64" s="42"/>
-      <c r="F64" s="42" t="s">
+      <c r="C64" s="144"/>
+      <c r="D64" s="144"/>
+      <c r="E64" s="144"/>
+      <c r="F64" s="144" t="s">
         <v>82</v>
       </c>
-      <c r="G64" s="42"/>
-      <c r="H64" s="42"/>
+      <c r="G64" s="144"/>
+      <c r="H64" s="144"/>
     </row>
     <row r="65" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="41" t="s">
+      <c r="B65" s="145" t="s">
         <v>83</v>
       </c>
-      <c r="C65" s="41"/>
-      <c r="D65" s="41"/>
-      <c r="E65" s="41"/>
-      <c r="F65" s="42" t="s">
+      <c r="C65" s="145"/>
+      <c r="D65" s="145"/>
+      <c r="E65" s="145"/>
+      <c r="F65" s="144" t="s">
         <v>84</v>
       </c>
-      <c r="G65" s="42"/>
-      <c r="H65" s="42"/>
+      <c r="G65" s="144"/>
+      <c r="H65" s="144"/>
     </row>
     <row r="66" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="41" t="s">
+      <c r="B66" s="145" t="s">
         <v>85</v>
       </c>
-      <c r="C66" s="41"/>
-      <c r="D66" s="41"/>
-      <c r="E66" s="41"/>
-      <c r="F66" s="42" t="s">
+      <c r="C66" s="145"/>
+      <c r="D66" s="145"/>
+      <c r="E66" s="145"/>
+      <c r="F66" s="144" t="s">
         <v>86</v>
       </c>
-      <c r="G66" s="42"/>
-      <c r="H66" s="42"/>
+      <c r="G66" s="144"/>
+      <c r="H66" s="144"/>
     </row>
     <row r="67" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="42" t="s">
+      <c r="B67" s="144" t="s">
         <v>87</v>
       </c>
-      <c r="C67" s="42"/>
-      <c r="D67" s="42"/>
-      <c r="E67" s="42"/>
-      <c r="F67" s="42"/>
-      <c r="G67" s="42"/>
+      <c r="C67" s="144"/>
+      <c r="D67" s="144"/>
+      <c r="E67" s="144"/>
+      <c r="F67" s="144"/>
+      <c r="G67" s="144"/>
     </row>
     <row r="68" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="39"/>
@@ -3056,12 +3006,75 @@
     <protectedRange algorithmName="SHA-512" hashValue="1IwEtpPovyRjspz9ti3J5udl070IPZ9gDlGmM3ZH/lFyQlLVVL2qbaMds7kHvZZkPq7VvowLV2MqpNnf8owpjQ==" saltValue="SwYyjj//I75seGLqQP0hyQ==" spinCount="100000" sqref="E37:G38 E39" name="Rango2_2"/>
   </protectedRanges>
   <mergeCells count="88">
-    <mergeCell ref="B9:G10"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="B66:E66"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="B62:G62"/>
+    <mergeCell ref="B63:G63"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="B56:G56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="B47:D49"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="C52:G52"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:G38"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B39:D40"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="E41:G42"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="B32:D33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="B35:D36"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:G24"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="E21:G21"/>
     <mergeCell ref="B11:E11"/>
@@ -3075,75 +3088,12 @@
     <mergeCell ref="E19:G19"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="E20:G20"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="B32:D33"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="B35:D36"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E37:G38"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B39:D40"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="E41:G42"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="B54:G54"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="B46:G46"/>
-    <mergeCell ref="B47:D49"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="C52:G52"/>
-    <mergeCell ref="B53:G53"/>
-    <mergeCell ref="B55:G55"/>
-    <mergeCell ref="B56:G56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:G58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="B62:G62"/>
-    <mergeCell ref="B63:G63"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="B66:E66"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="B9:G10"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="A8:H8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D7" r:id="rId1" xr:uid="{06F8AEE0-B467-46CC-BA80-3945E484B37D}"/>

</xml_diff>